<commit_message>
Broken pieces and not tools are excluded, and some catalog numbers are adjusted based on Dietz's data.
</commit_message>
<xml_diff>
--- a/data/Caliper_ImageJ_comparison.xlsx
+++ b/data/Caliper_ImageJ_comparison.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FilesVC\GMM-exp-boxgrove-gona\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5637D72-50AA-4498-9026-52267CCB3E0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA75792-C606-483E-A238-53E95C0D35A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="52">
   <si>
     <t>site</t>
   </si>
@@ -515,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG48"/>
+  <dimension ref="A1:AG37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A48"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -730,64 +731,100 @@
         <v>19</v>
       </c>
       <c r="B3">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3">
+        <v>181</v>
+      </c>
+      <c r="G3">
+        <v>79.5</v>
+      </c>
+      <c r="H3">
+        <v>64</v>
+      </c>
+      <c r="I3">
+        <v>77</v>
+      </c>
+      <c r="J3">
+        <v>61.87</v>
+      </c>
+      <c r="K3">
+        <v>29.37</v>
+      </c>
+      <c r="L3">
+        <v>63</v>
+      </c>
+      <c r="M3">
+        <v>61</v>
+      </c>
+      <c r="N3">
+        <v>35.880000000000003</v>
       </c>
       <c r="O3">
-        <v>97.23</v>
+        <v>188.4</v>
       </c>
       <c r="P3">
-        <v>12.593</v>
+        <v>22.37</v>
       </c>
       <c r="Q3">
-        <v>16.84</v>
+        <v>32.938000000000002</v>
       </c>
       <c r="R3">
-        <v>23.704000000000001</v>
+        <v>42.716000000000001</v>
       </c>
       <c r="S3">
-        <v>29.777999999999999</v>
+        <v>49.63</v>
       </c>
       <c r="T3">
-        <v>35.308999999999997</v>
+        <v>55.802</v>
       </c>
       <c r="U3">
-        <v>41.926000000000002</v>
+        <v>56.79</v>
       </c>
       <c r="V3">
-        <v>50.37</v>
+        <v>60.345999999999997</v>
       </c>
       <c r="W3">
-        <v>43.802</v>
+        <v>67.16</v>
       </c>
       <c r="X3">
-        <v>24.937999999999999</v>
+        <v>60.84</v>
       </c>
       <c r="Y3">
-        <v>14.519</v>
+        <v>19.951000000000001</v>
       </c>
       <c r="Z3">
-        <v>24.295999999999999</v>
+        <v>26.37</v>
       </c>
       <c r="AA3">
-        <v>32.889000000000003</v>
+        <v>39.802</v>
       </c>
       <c r="AB3">
-        <v>38.914000000000001</v>
+        <v>48.198</v>
       </c>
       <c r="AC3">
-        <v>43.061999999999998</v>
+        <v>67.358000000000004</v>
       </c>
       <c r="AD3">
-        <v>46.024999999999999</v>
+        <v>70.962999999999994</v>
       </c>
       <c r="AE3">
-        <v>49.530999999999999</v>
+        <v>77.480999999999995</v>
       </c>
       <c r="AF3">
-        <v>55.753</v>
+        <v>74.320999999999998</v>
       </c>
       <c r="AG3">
-        <v>63.259</v>
+        <v>64.197999999999993</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.45">
@@ -795,6 +832,3719 @@
         <v>19</v>
       </c>
       <c r="B4">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4">
+        <v>156</v>
+      </c>
+      <c r="G4">
+        <v>88</v>
+      </c>
+      <c r="H4">
+        <v>80</v>
+      </c>
+      <c r="I4">
+        <v>62.49</v>
+      </c>
+      <c r="J4">
+        <v>88</v>
+      </c>
+      <c r="K4">
+        <v>50.38</v>
+      </c>
+      <c r="L4">
+        <v>46.55</v>
+      </c>
+      <c r="M4">
+        <v>78.040000000000006</v>
+      </c>
+      <c r="N4">
+        <v>39.53</v>
+      </c>
+      <c r="O4">
+        <v>159.01</v>
+      </c>
+      <c r="P4">
+        <v>40.345999999999997</v>
+      </c>
+      <c r="Q4">
+        <v>53.777999999999999</v>
+      </c>
+      <c r="R4">
+        <v>65.826999999999998</v>
+      </c>
+      <c r="S4">
+        <v>72.444000000000003</v>
+      </c>
+      <c r="T4">
+        <v>81.679000000000002</v>
+      </c>
+      <c r="U4">
+        <v>91.406999999999996</v>
+      </c>
+      <c r="V4">
+        <v>79.010000000000005</v>
+      </c>
+      <c r="W4">
+        <v>59.457000000000001</v>
+      </c>
+      <c r="X4">
+        <v>38.271999999999998</v>
+      </c>
+      <c r="Y4">
+        <v>33.728000000000002</v>
+      </c>
+      <c r="Z4">
+        <v>48.889000000000003</v>
+      </c>
+      <c r="AA4">
+        <v>62.469000000000001</v>
+      </c>
+      <c r="AB4">
+        <v>81.037000000000006</v>
+      </c>
+      <c r="AC4">
+        <v>91.406999999999996</v>
+      </c>
+      <c r="AD4">
+        <v>97.432000000000002</v>
+      </c>
+      <c r="AE4">
+        <v>91.703999999999994</v>
+      </c>
+      <c r="AF4">
+        <v>76.84</v>
+      </c>
+      <c r="AG4">
+        <v>57.68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1">
+        <v>34</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="1">
+        <v>141</v>
+      </c>
+      <c r="G5" s="1">
+        <v>81</v>
+      </c>
+      <c r="H5" s="1">
+        <v>56</v>
+      </c>
+      <c r="I5" s="1">
+        <v>75.5</v>
+      </c>
+      <c r="J5" s="1">
+        <v>61.62</v>
+      </c>
+      <c r="K5" s="1">
+        <v>40.75</v>
+      </c>
+      <c r="L5" s="1">
+        <v>54.17</v>
+      </c>
+      <c r="M5" s="1">
+        <v>56</v>
+      </c>
+      <c r="N5" s="1">
+        <v>30.08</v>
+      </c>
+      <c r="O5" s="1">
+        <v>147.06</v>
+      </c>
+      <c r="P5" s="1">
+        <v>20.641999999999999</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>28.395</v>
+      </c>
+      <c r="R5" s="1">
+        <v>37.036999999999999</v>
+      </c>
+      <c r="S5" s="1">
+        <v>49.975000000000001</v>
+      </c>
+      <c r="T5" s="1">
+        <v>56.889000000000003</v>
+      </c>
+      <c r="U5" s="1">
+        <v>63.110999999999997</v>
+      </c>
+      <c r="V5" s="1">
+        <v>61.777999999999999</v>
+      </c>
+      <c r="W5" s="1">
+        <v>57.085999999999999</v>
+      </c>
+      <c r="X5" s="1">
+        <v>44.84</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>18.914000000000001</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>32.048999999999999</v>
+      </c>
+      <c r="AA5" s="1">
+        <v>49.283999999999999</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>58.122999999999998</v>
+      </c>
+      <c r="AC5" s="1">
+        <v>68.84</v>
+      </c>
+      <c r="AD5" s="1">
+        <v>77.778000000000006</v>
+      </c>
+      <c r="AE5" s="1">
+        <v>83.406999999999996</v>
+      </c>
+      <c r="AF5" s="1">
+        <v>74.765000000000001</v>
+      </c>
+      <c r="AG5" s="1">
+        <v>57.481000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6">
+        <v>117</v>
+      </c>
+      <c r="G6">
+        <v>84</v>
+      </c>
+      <c r="H6">
+        <v>55</v>
+      </c>
+      <c r="I6">
+        <v>85.11</v>
+      </c>
+      <c r="J6">
+        <v>76.64</v>
+      </c>
+      <c r="K6">
+        <v>34.130000000000003</v>
+      </c>
+      <c r="L6">
+        <v>53.24</v>
+      </c>
+      <c r="M6">
+        <v>53.07</v>
+      </c>
+      <c r="N6">
+        <v>34.42</v>
+      </c>
+      <c r="O6">
+        <v>125.33</v>
+      </c>
+      <c r="P6">
+        <v>20.741</v>
+      </c>
+      <c r="Q6">
+        <v>29.678999999999998</v>
+      </c>
+      <c r="R6">
+        <v>43.802</v>
+      </c>
+      <c r="S6">
+        <v>55.604999999999997</v>
+      </c>
+      <c r="T6">
+        <v>60.494</v>
+      </c>
+      <c r="U6">
+        <v>63.110999999999997</v>
+      </c>
+      <c r="V6">
+        <v>62.271999999999998</v>
+      </c>
+      <c r="W6">
+        <v>58.567999999999998</v>
+      </c>
+      <c r="X6">
+        <v>41.085999999999999</v>
+      </c>
+      <c r="Y6">
+        <v>16.79</v>
+      </c>
+      <c r="Z6">
+        <v>29.63</v>
+      </c>
+      <c r="AA6">
+        <v>45.63</v>
+      </c>
+      <c r="AB6">
+        <v>66.221999999999994</v>
+      </c>
+      <c r="AC6">
+        <v>79.012</v>
+      </c>
+      <c r="AD6">
+        <v>85.876999999999995</v>
+      </c>
+      <c r="AE6">
+        <v>87.950999999999993</v>
+      </c>
+      <c r="AF6">
+        <v>86.567999999999998</v>
+      </c>
+      <c r="AG6">
+        <v>77.135999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7">
+        <v>103</v>
+      </c>
+      <c r="G7">
+        <v>58</v>
+      </c>
+      <c r="H7">
+        <v>47</v>
+      </c>
+      <c r="I7">
+        <v>57.64</v>
+      </c>
+      <c r="J7">
+        <v>51.18</v>
+      </c>
+      <c r="K7">
+        <v>30.81</v>
+      </c>
+      <c r="L7">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="M7">
+        <v>43.6</v>
+      </c>
+      <c r="N7">
+        <v>24.55</v>
+      </c>
+      <c r="O7">
+        <v>108.2</v>
+      </c>
+      <c r="P7">
+        <v>11.654</v>
+      </c>
+      <c r="Q7">
+        <v>18.222000000000001</v>
+      </c>
+      <c r="R7">
+        <v>23.111000000000001</v>
+      </c>
+      <c r="S7">
+        <v>31.259</v>
+      </c>
+      <c r="T7">
+        <v>40.395000000000003</v>
+      </c>
+      <c r="U7">
+        <v>51.16</v>
+      </c>
+      <c r="V7">
+        <v>48.048999999999999</v>
+      </c>
+      <c r="W7">
+        <v>37.234999999999999</v>
+      </c>
+      <c r="X7">
+        <v>27.062000000000001</v>
+      </c>
+      <c r="Y7">
+        <v>18.024999999999999</v>
+      </c>
+      <c r="Z7">
+        <v>24.79</v>
+      </c>
+      <c r="AA7">
+        <v>31.704000000000001</v>
+      </c>
+      <c r="AB7">
+        <v>42.122999999999998</v>
+      </c>
+      <c r="AC7">
+        <v>51.604999999999997</v>
+      </c>
+      <c r="AD7">
+        <v>52.988</v>
+      </c>
+      <c r="AE7">
+        <v>57.777999999999999</v>
+      </c>
+      <c r="AF7">
+        <v>60.148000000000003</v>
+      </c>
+      <c r="AG7">
+        <v>49.777999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>201</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8">
+        <v>125</v>
+      </c>
+      <c r="G8">
+        <v>75.099999999999994</v>
+      </c>
+      <c r="H8">
+        <v>34.5</v>
+      </c>
+      <c r="I8">
+        <v>75.3</v>
+      </c>
+      <c r="J8">
+        <v>68.7</v>
+      </c>
+      <c r="K8">
+        <v>62.2</v>
+      </c>
+      <c r="L8">
+        <v>22</v>
+      </c>
+      <c r="M8">
+        <v>28.3</v>
+      </c>
+      <c r="N8">
+        <v>33</v>
+      </c>
+      <c r="O8">
+        <v>133.19</v>
+      </c>
+      <c r="P8">
+        <v>33.283999999999999</v>
+      </c>
+      <c r="Q8">
+        <v>41.975000000000001</v>
+      </c>
+      <c r="R8">
+        <v>41.826999999999998</v>
+      </c>
+      <c r="S8">
+        <v>43.506</v>
+      </c>
+      <c r="T8">
+        <v>47.357999999999997</v>
+      </c>
+      <c r="U8">
+        <v>47.604999999999997</v>
+      </c>
+      <c r="V8">
+        <v>46.222000000000001</v>
+      </c>
+      <c r="W8">
+        <v>44</v>
+      </c>
+      <c r="X8">
+        <v>38.667000000000002</v>
+      </c>
+      <c r="Y8">
+        <v>41.63</v>
+      </c>
+      <c r="Z8">
+        <v>66.272000000000006</v>
+      </c>
+      <c r="AA8">
+        <v>72</v>
+      </c>
+      <c r="AB8">
+        <v>72.346000000000004</v>
+      </c>
+      <c r="AC8">
+        <v>68.938000000000002</v>
+      </c>
+      <c r="AD8">
+        <v>75.061999999999998</v>
+      </c>
+      <c r="AE8">
+        <v>76.888999999999996</v>
+      </c>
+      <c r="AF8">
+        <v>74.42</v>
+      </c>
+      <c r="AG8">
+        <v>64.049000000000007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>231</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9">
+        <v>101</v>
+      </c>
+      <c r="G9">
+        <v>90</v>
+      </c>
+      <c r="H9">
+        <v>63</v>
+      </c>
+      <c r="I9">
+        <v>68.150000000000006</v>
+      </c>
+      <c r="J9">
+        <v>75.23</v>
+      </c>
+      <c r="K9">
+        <v>41.79</v>
+      </c>
+      <c r="L9">
+        <v>50.37</v>
+      </c>
+      <c r="M9">
+        <v>58.29</v>
+      </c>
+      <c r="N9">
+        <v>46.03</v>
+      </c>
+      <c r="O9">
+        <v>103.94999999999999</v>
+      </c>
+      <c r="P9">
+        <v>29.332999999999998</v>
+      </c>
+      <c r="Q9">
+        <v>43.802</v>
+      </c>
+      <c r="R9">
+        <v>56.988</v>
+      </c>
+      <c r="S9">
+        <v>60.84</v>
+      </c>
+      <c r="T9">
+        <v>64.790000000000006</v>
+      </c>
+      <c r="U9">
+        <v>65.382999999999996</v>
+      </c>
+      <c r="V9">
+        <v>60.741</v>
+      </c>
+      <c r="W9">
+        <v>50.173000000000002</v>
+      </c>
+      <c r="X9">
+        <v>33.432000000000002</v>
+      </c>
+      <c r="Y9">
+        <v>38.122999999999998</v>
+      </c>
+      <c r="Z9">
+        <v>53.481000000000002</v>
+      </c>
+      <c r="AA9">
+        <v>59.357999999999997</v>
+      </c>
+      <c r="AB9">
+        <v>73.826999999999998</v>
+      </c>
+      <c r="AC9">
+        <v>86.025000000000006</v>
+      </c>
+      <c r="AD9">
+        <v>87.802000000000007</v>
+      </c>
+      <c r="AE9">
+        <v>73.778000000000006</v>
+      </c>
+      <c r="AF9">
+        <v>61.332999999999998</v>
+      </c>
+      <c r="AG9">
+        <v>39.700000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10">
+        <v>1125</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10">
+        <v>85.3</v>
+      </c>
+      <c r="G10">
+        <v>65.8</v>
+      </c>
+      <c r="H10">
+        <v>35</v>
+      </c>
+      <c r="I10">
+        <v>56.6</v>
+      </c>
+      <c r="J10">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="K10">
+        <v>54.1</v>
+      </c>
+      <c r="L10">
+        <v>26.2</v>
+      </c>
+      <c r="M10">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="N10">
+        <v>24.4</v>
+      </c>
+      <c r="O10">
+        <v>77.42</v>
+      </c>
+      <c r="P10">
+        <v>18.582999999999998</v>
+      </c>
+      <c r="Q10">
+        <v>25.75</v>
+      </c>
+      <c r="R10">
+        <v>29.542000000000002</v>
+      </c>
+      <c r="S10">
+        <v>34.667000000000002</v>
+      </c>
+      <c r="T10">
+        <v>37.082999999999998</v>
+      </c>
+      <c r="U10">
+        <v>37.707999999999998</v>
+      </c>
+      <c r="V10">
+        <v>35.082999999999998</v>
+      </c>
+      <c r="W10">
+        <v>31.167000000000002</v>
+      </c>
+      <c r="X10">
+        <v>25.792000000000002</v>
+      </c>
+      <c r="Y10">
+        <v>34.738999999999997</v>
+      </c>
+      <c r="Z10">
+        <v>47.042999999999999</v>
+      </c>
+      <c r="AA10">
+        <v>61.652000000000001</v>
+      </c>
+      <c r="AB10">
+        <v>64.912999999999997</v>
+      </c>
+      <c r="AC10">
+        <v>66.260999999999996</v>
+      </c>
+      <c r="AD10">
+        <v>64.912999999999997</v>
+      </c>
+      <c r="AE10">
+        <v>61.87</v>
+      </c>
+      <c r="AF10">
+        <v>50.738999999999997</v>
+      </c>
+      <c r="AG10">
+        <v>34.783000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11">
+        <v>1184</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11">
+        <v>104.7</v>
+      </c>
+      <c r="G11">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="H11">
+        <v>50.8</v>
+      </c>
+      <c r="I11">
+        <v>45.7</v>
+      </c>
+      <c r="J11">
+        <v>67.2</v>
+      </c>
+      <c r="K11">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="L11">
+        <v>38.700000000000003</v>
+      </c>
+      <c r="M11">
+        <v>48.3</v>
+      </c>
+      <c r="N11">
+        <v>41.7</v>
+      </c>
+      <c r="O11">
+        <v>102.25</v>
+      </c>
+      <c r="P11">
+        <v>14.628</v>
+      </c>
+      <c r="Q11">
+        <v>32.975000000000001</v>
+      </c>
+      <c r="R11">
+        <v>50.744</v>
+      </c>
+      <c r="S11">
+        <v>60.164999999999999</v>
+      </c>
+      <c r="T11">
+        <v>63.802</v>
+      </c>
+      <c r="U11">
+        <v>60.247999999999998</v>
+      </c>
+      <c r="V11">
+        <v>55.124000000000002</v>
+      </c>
+      <c r="W11">
+        <v>41.156999999999996</v>
+      </c>
+      <c r="X11">
+        <v>24.297999999999998</v>
+      </c>
+      <c r="Y11">
+        <v>26.5</v>
+      </c>
+      <c r="Z11">
+        <v>39.542000000000002</v>
+      </c>
+      <c r="AA11">
+        <v>46.042000000000002</v>
+      </c>
+      <c r="AB11">
+        <v>49.707999999999998</v>
+      </c>
+      <c r="AC11">
+        <v>52.207999999999998</v>
+      </c>
+      <c r="AD11">
+        <v>53.042000000000002</v>
+      </c>
+      <c r="AE11">
+        <v>51.5</v>
+      </c>
+      <c r="AF11">
+        <v>43.875</v>
+      </c>
+      <c r="AG11">
+        <v>27.207999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <v>1223</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12">
+        <v>82</v>
+      </c>
+      <c r="G12">
+        <v>57.7</v>
+      </c>
+      <c r="H12">
+        <v>38.9</v>
+      </c>
+      <c r="I12">
+        <v>50.4</v>
+      </c>
+      <c r="J12">
+        <v>57.1</v>
+      </c>
+      <c r="K12">
+        <v>48.5</v>
+      </c>
+      <c r="L12">
+        <v>26.9</v>
+      </c>
+      <c r="M12">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="O12">
+        <v>81.820000000000007</v>
+      </c>
+      <c r="P12">
+        <v>12.241</v>
+      </c>
+      <c r="Q12">
+        <v>20.776</v>
+      </c>
+      <c r="R12">
+        <v>31.466000000000001</v>
+      </c>
+      <c r="S12">
+        <v>41.25</v>
+      </c>
+      <c r="T12">
+        <v>42.112000000000002</v>
+      </c>
+      <c r="U12">
+        <v>42.026000000000003</v>
+      </c>
+      <c r="V12">
+        <v>38.146999999999998</v>
+      </c>
+      <c r="W12">
+        <v>32.5</v>
+      </c>
+      <c r="X12">
+        <v>25.603000000000002</v>
+      </c>
+      <c r="Y12">
+        <v>26.489000000000001</v>
+      </c>
+      <c r="Z12">
+        <v>45.689</v>
+      </c>
+      <c r="AA12">
+        <v>51.822000000000003</v>
+      </c>
+      <c r="AB12">
+        <v>54.311</v>
+      </c>
+      <c r="AC12">
+        <v>55.289000000000001</v>
+      </c>
+      <c r="AD12">
+        <v>53.155999999999999</v>
+      </c>
+      <c r="AE12">
+        <v>48.844000000000001</v>
+      </c>
+      <c r="AF12">
+        <v>43.244</v>
+      </c>
+      <c r="AG12">
+        <v>33.421999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>1320</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13">
+        <v>81.2</v>
+      </c>
+      <c r="G13">
+        <v>66.8</v>
+      </c>
+      <c r="H13">
+        <v>59.6</v>
+      </c>
+      <c r="I13">
+        <v>62.8</v>
+      </c>
+      <c r="J13">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="K13">
+        <v>50.9</v>
+      </c>
+      <c r="L13">
+        <v>57.4</v>
+      </c>
+      <c r="M13">
+        <v>59.6</v>
+      </c>
+      <c r="N13">
+        <v>52.4</v>
+      </c>
+      <c r="O13">
+        <v>80.55</v>
+      </c>
+      <c r="P13">
+        <v>40.167000000000002</v>
+      </c>
+      <c r="Q13">
+        <v>48.536000000000001</v>
+      </c>
+      <c r="R13">
+        <v>52.802999999999997</v>
+      </c>
+      <c r="S13">
+        <v>55.23</v>
+      </c>
+      <c r="T13">
+        <v>56.987000000000002</v>
+      </c>
+      <c r="U13">
+        <v>55.314</v>
+      </c>
+      <c r="V13">
+        <v>52.05</v>
+      </c>
+      <c r="W13">
+        <v>48.451999999999998</v>
+      </c>
+      <c r="X13">
+        <v>43.472999999999999</v>
+      </c>
+      <c r="Y13">
+        <v>27.553000000000001</v>
+      </c>
+      <c r="Z13">
+        <v>49.494</v>
+      </c>
+      <c r="AA13">
+        <v>58.143000000000001</v>
+      </c>
+      <c r="AB13">
+        <v>62.743000000000002</v>
+      </c>
+      <c r="AC13">
+        <v>67.215000000000003</v>
+      </c>
+      <c r="AD13">
+        <v>67.468000000000004</v>
+      </c>
+      <c r="AE13">
+        <v>62.658000000000001</v>
+      </c>
+      <c r="AF13">
+        <v>56.286999999999999</v>
+      </c>
+      <c r="AG13">
+        <v>42.024999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>1559</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14">
+        <v>80</v>
+      </c>
+      <c r="G14">
+        <v>56.3</v>
+      </c>
+      <c r="H14">
+        <v>34.6</v>
+      </c>
+      <c r="I14">
+        <v>52.1</v>
+      </c>
+      <c r="J14">
+        <v>49.8</v>
+      </c>
+      <c r="K14">
+        <v>44.8</v>
+      </c>
+      <c r="L14">
+        <v>34.4</v>
+      </c>
+      <c r="M14">
+        <v>34.5</v>
+      </c>
+      <c r="N14">
+        <v>33.5</v>
+      </c>
+      <c r="O14">
+        <v>78.09</v>
+      </c>
+      <c r="P14">
+        <v>22.92</v>
+      </c>
+      <c r="Q14">
+        <v>30.12</v>
+      </c>
+      <c r="R14">
+        <v>33.28</v>
+      </c>
+      <c r="S14">
+        <v>33.96</v>
+      </c>
+      <c r="T14">
+        <v>34.28</v>
+      </c>
+      <c r="U14">
+        <v>34.08</v>
+      </c>
+      <c r="V14">
+        <v>33.880000000000003</v>
+      </c>
+      <c r="W14">
+        <v>33.880000000000003</v>
+      </c>
+      <c r="X14">
+        <v>30.32</v>
+      </c>
+      <c r="Y14">
+        <v>24.489000000000001</v>
+      </c>
+      <c r="Z14">
+        <v>41.732999999999997</v>
+      </c>
+      <c r="AA14">
+        <v>49.2</v>
+      </c>
+      <c r="AB14">
+        <v>56.488999999999997</v>
+      </c>
+      <c r="AC14">
+        <v>60.267000000000003</v>
+      </c>
+      <c r="AD14">
+        <v>59.421999999999997</v>
+      </c>
+      <c r="AE14">
+        <v>51.777999999999999</v>
+      </c>
+      <c r="AF14">
+        <v>38.889000000000003</v>
+      </c>
+      <c r="AG14">
+        <v>23.733000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>2002</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15">
+        <v>46</v>
+      </c>
+      <c r="G15">
+        <v>38</v>
+      </c>
+      <c r="H15">
+        <v>32</v>
+      </c>
+      <c r="I15">
+        <v>35.6</v>
+      </c>
+      <c r="J15">
+        <v>37.5</v>
+      </c>
+      <c r="K15">
+        <v>31.6</v>
+      </c>
+      <c r="L15">
+        <v>26.7</v>
+      </c>
+      <c r="M15">
+        <v>31</v>
+      </c>
+      <c r="N15">
+        <v>26.9</v>
+      </c>
+      <c r="O15">
+        <v>48.16</v>
+      </c>
+      <c r="P15">
+        <v>16.706</v>
+      </c>
+      <c r="Q15">
+        <v>24.869</v>
+      </c>
+      <c r="R15">
+        <v>28.222000000000001</v>
+      </c>
+      <c r="S15">
+        <v>30.728999999999999</v>
+      </c>
+      <c r="T15">
+        <v>31.137</v>
+      </c>
+      <c r="U15">
+        <v>32.156999999999996</v>
+      </c>
+      <c r="V15">
+        <v>34.869</v>
+      </c>
+      <c r="W15">
+        <v>30.321000000000002</v>
+      </c>
+      <c r="X15">
+        <v>20.233000000000001</v>
+      </c>
+      <c r="Y15">
+        <v>27.318000000000001</v>
+      </c>
+      <c r="Z15">
+        <v>31.545000000000002</v>
+      </c>
+      <c r="AA15">
+        <v>33.293999999999997</v>
+      </c>
+      <c r="AB15">
+        <v>36.792999999999999</v>
+      </c>
+      <c r="AC15">
+        <v>38.570999999999998</v>
+      </c>
+      <c r="AD15">
+        <v>37.405000000000001</v>
+      </c>
+      <c r="AE15">
+        <v>35.948</v>
+      </c>
+      <c r="AF15">
+        <v>34.344000000000001</v>
+      </c>
+      <c r="AG15">
+        <v>26.617999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16">
+        <v>2006</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16">
+        <v>42</v>
+      </c>
+      <c r="G16">
+        <v>34</v>
+      </c>
+      <c r="H16">
+        <v>16</v>
+      </c>
+      <c r="I16">
+        <v>29.8</v>
+      </c>
+      <c r="J16">
+        <v>31.3</v>
+      </c>
+      <c r="K16">
+        <v>27.1</v>
+      </c>
+      <c r="L16">
+        <v>13.9</v>
+      </c>
+      <c r="M16">
+        <v>15.2</v>
+      </c>
+      <c r="N16">
+        <v>13.1</v>
+      </c>
+      <c r="O16">
+        <v>43.58</v>
+      </c>
+      <c r="P16">
+        <v>5.7539999999999996</v>
+      </c>
+      <c r="Q16">
+        <v>12.316000000000001</v>
+      </c>
+      <c r="R16">
+        <v>16.07</v>
+      </c>
+      <c r="S16">
+        <v>17.965</v>
+      </c>
+      <c r="T16">
+        <v>18.315999999999999</v>
+      </c>
+      <c r="U16">
+        <v>18.105</v>
+      </c>
+      <c r="V16">
+        <v>17.684000000000001</v>
+      </c>
+      <c r="W16">
+        <v>16.07</v>
+      </c>
+      <c r="X16">
+        <v>12.175000000000001</v>
+      </c>
+      <c r="Y16">
+        <v>23.509</v>
+      </c>
+      <c r="Z16">
+        <v>28.911999999999999</v>
+      </c>
+      <c r="AA16">
+        <v>30.596</v>
+      </c>
+      <c r="AB16">
+        <v>33.228000000000002</v>
+      </c>
+      <c r="AC16">
+        <v>32.350999999999999</v>
+      </c>
+      <c r="AD16">
+        <v>31.123000000000001</v>
+      </c>
+      <c r="AE16">
+        <v>29.439</v>
+      </c>
+      <c r="AF16">
+        <v>27.367999999999999</v>
+      </c>
+      <c r="AG16">
+        <v>25.544</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17">
+        <v>2016</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17">
+        <v>73</v>
+      </c>
+      <c r="G17">
+        <v>49</v>
+      </c>
+      <c r="H17">
+        <v>46</v>
+      </c>
+      <c r="I17">
+        <v>41.3</v>
+      </c>
+      <c r="J17">
+        <v>41.6</v>
+      </c>
+      <c r="K17">
+        <v>28.3</v>
+      </c>
+      <c r="L17">
+        <v>14.7</v>
+      </c>
+      <c r="M17">
+        <v>25</v>
+      </c>
+      <c r="N17">
+        <v>14.2</v>
+      </c>
+      <c r="O17">
+        <v>79.710000000000008</v>
+      </c>
+      <c r="P17">
+        <v>14.84</v>
+      </c>
+      <c r="Q17">
+        <v>21.37</v>
+      </c>
+      <c r="R17">
+        <v>27.725999999999999</v>
+      </c>
+      <c r="S17">
+        <v>32.478000000000002</v>
+      </c>
+      <c r="T17">
+        <v>37.872</v>
+      </c>
+      <c r="U17">
+        <v>44.402000000000001</v>
+      </c>
+      <c r="V17">
+        <v>48.892000000000003</v>
+      </c>
+      <c r="W17">
+        <v>51.223999999999997</v>
+      </c>
+      <c r="X17">
+        <v>44.636000000000003</v>
+      </c>
+      <c r="Y17">
+        <v>20.350000000000001</v>
+      </c>
+      <c r="Z17">
+        <v>27.492999999999999</v>
+      </c>
+      <c r="AA17">
+        <v>32.594999999999999</v>
+      </c>
+      <c r="AB17">
+        <v>38.250999999999998</v>
+      </c>
+      <c r="AC17">
+        <v>48.192</v>
+      </c>
+      <c r="AD17">
+        <v>53.12</v>
+      </c>
+      <c r="AE17">
+        <v>52.012</v>
+      </c>
+      <c r="AF17">
+        <v>50.146000000000001</v>
+      </c>
+      <c r="AG17">
+        <v>38.22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>2066</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18">
+        <v>44</v>
+      </c>
+      <c r="G18">
+        <v>33</v>
+      </c>
+      <c r="H18">
+        <v>27</v>
+      </c>
+      <c r="I18">
+        <v>29.8</v>
+      </c>
+      <c r="J18">
+        <v>28.3</v>
+      </c>
+      <c r="K18">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="L18">
+        <v>25.2</v>
+      </c>
+      <c r="M18">
+        <v>25.4</v>
+      </c>
+      <c r="N18">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="O18">
+        <v>45.129999999999995</v>
+      </c>
+      <c r="P18">
+        <v>11.603</v>
+      </c>
+      <c r="Q18">
+        <v>15.16</v>
+      </c>
+      <c r="R18">
+        <v>18.251000000000001</v>
+      </c>
+      <c r="S18">
+        <v>22.187000000000001</v>
+      </c>
+      <c r="T18">
+        <v>25.044</v>
+      </c>
+      <c r="U18">
+        <v>28.28</v>
+      </c>
+      <c r="V18">
+        <v>31.195</v>
+      </c>
+      <c r="W18">
+        <v>33.090000000000003</v>
+      </c>
+      <c r="X18">
+        <v>32.186999999999998</v>
+      </c>
+      <c r="Y18">
+        <v>12.65</v>
+      </c>
+      <c r="Z18">
+        <v>18.076000000000001</v>
+      </c>
+      <c r="AA18">
+        <v>19.649999999999999</v>
+      </c>
+      <c r="AB18">
+        <v>20</v>
+      </c>
+      <c r="AC18">
+        <v>23.994</v>
+      </c>
+      <c r="AD18">
+        <v>27.93</v>
+      </c>
+      <c r="AE18">
+        <v>29.738</v>
+      </c>
+      <c r="AF18">
+        <v>30.117000000000001</v>
+      </c>
+      <c r="AG18">
+        <v>25.19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>2081</v>
+      </c>
+      <c r="C19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19">
+        <v>47</v>
+      </c>
+      <c r="G19">
+        <v>38</v>
+      </c>
+      <c r="H19">
+        <v>25</v>
+      </c>
+      <c r="I19">
+        <v>37.5</v>
+      </c>
+      <c r="J19">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="K19">
+        <v>23.8</v>
+      </c>
+      <c r="L19">
+        <v>25.4</v>
+      </c>
+      <c r="M19">
+        <v>23.3</v>
+      </c>
+      <c r="N19">
+        <v>18</v>
+      </c>
+      <c r="O19">
+        <v>44.960000000000008</v>
+      </c>
+      <c r="P19">
+        <v>15.218999999999999</v>
+      </c>
+      <c r="Q19">
+        <v>19.359000000000002</v>
+      </c>
+      <c r="R19">
+        <v>22.710999999999999</v>
+      </c>
+      <c r="S19">
+        <v>27.143000000000001</v>
+      </c>
+      <c r="T19">
+        <v>29.3</v>
+      </c>
+      <c r="U19">
+        <v>29.853999999999999</v>
+      </c>
+      <c r="V19">
+        <v>28.192</v>
+      </c>
+      <c r="W19">
+        <v>24.547999999999998</v>
+      </c>
+      <c r="X19">
+        <v>16.268000000000001</v>
+      </c>
+      <c r="Y19">
+        <v>22.157</v>
+      </c>
+      <c r="Z19">
+        <v>31.777999999999999</v>
+      </c>
+      <c r="AA19">
+        <v>33.527999999999999</v>
+      </c>
+      <c r="AB19">
+        <v>34.14</v>
+      </c>
+      <c r="AC19">
+        <v>35.889000000000003</v>
+      </c>
+      <c r="AD19">
+        <v>37.637999999999998</v>
+      </c>
+      <c r="AE19">
+        <v>39.095999999999997</v>
+      </c>
+      <c r="AF19">
+        <v>36.064</v>
+      </c>
+      <c r="AG19">
+        <v>29.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20">
+        <v>2092</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20">
+        <v>41</v>
+      </c>
+      <c r="G20">
+        <v>33.1</v>
+      </c>
+      <c r="H20">
+        <v>26</v>
+      </c>
+      <c r="I20">
+        <v>24.3</v>
+      </c>
+      <c r="J20">
+        <v>31.3</v>
+      </c>
+      <c r="K20">
+        <v>21.3</v>
+      </c>
+      <c r="L20">
+        <v>22</v>
+      </c>
+      <c r="M20">
+        <v>24.7</v>
+      </c>
+      <c r="N20">
+        <v>22</v>
+      </c>
+      <c r="O20">
+        <v>42.35</v>
+      </c>
+      <c r="P20">
+        <v>15.474</v>
+      </c>
+      <c r="Q20">
+        <v>21.228000000000002</v>
+      </c>
+      <c r="R20">
+        <v>25.93</v>
+      </c>
+      <c r="S20">
+        <v>27.719000000000001</v>
+      </c>
+      <c r="T20">
+        <v>27.332999999999998</v>
+      </c>
+      <c r="U20">
+        <v>27.367999999999999</v>
+      </c>
+      <c r="V20">
+        <v>27.544</v>
+      </c>
+      <c r="W20">
+        <v>26.946999999999999</v>
+      </c>
+      <c r="X20">
+        <v>26.105</v>
+      </c>
+      <c r="Y20">
+        <v>16.175000000000001</v>
+      </c>
+      <c r="Z20">
+        <v>20.876999999999999</v>
+      </c>
+      <c r="AA20">
+        <v>25.719000000000001</v>
+      </c>
+      <c r="AB20">
+        <v>29.053000000000001</v>
+      </c>
+      <c r="AC20">
+        <v>30.491</v>
+      </c>
+      <c r="AD20">
+        <v>29.193000000000001</v>
+      </c>
+      <c r="AE20">
+        <v>28.210999999999999</v>
+      </c>
+      <c r="AF20">
+        <v>26.667000000000002</v>
+      </c>
+      <c r="AG20">
+        <v>20.526</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21">
+        <v>2114</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21">
+        <v>49</v>
+      </c>
+      <c r="G21">
+        <v>39</v>
+      </c>
+      <c r="H21">
+        <v>38</v>
+      </c>
+      <c r="I21">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="J21">
+        <v>30.9</v>
+      </c>
+      <c r="K21">
+        <v>27.7</v>
+      </c>
+      <c r="L21">
+        <v>30.4</v>
+      </c>
+      <c r="M21">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="N21">
+        <v>21.3</v>
+      </c>
+      <c r="O21">
+        <v>50.25</v>
+      </c>
+      <c r="P21">
+        <v>16.491</v>
+      </c>
+      <c r="Q21">
+        <v>22.315999999999999</v>
+      </c>
+      <c r="R21">
+        <v>26.876999999999999</v>
+      </c>
+      <c r="S21">
+        <v>30.946999999999999</v>
+      </c>
+      <c r="T21">
+        <v>34.737000000000002</v>
+      </c>
+      <c r="U21">
+        <v>35.543999999999997</v>
+      </c>
+      <c r="V21">
+        <v>35.683999999999997</v>
+      </c>
+      <c r="W21">
+        <v>34.174999999999997</v>
+      </c>
+      <c r="X21">
+        <v>33.789000000000001</v>
+      </c>
+      <c r="Y21">
+        <v>12.420999999999999</v>
+      </c>
+      <c r="Z21">
+        <v>26.280999999999999</v>
+      </c>
+      <c r="AA21">
+        <v>29.614000000000001</v>
+      </c>
+      <c r="AB21">
+        <v>31.053000000000001</v>
+      </c>
+      <c r="AC21">
+        <v>35.332999999999998</v>
+      </c>
+      <c r="AD21">
+        <v>40.316000000000003</v>
+      </c>
+      <c r="AE21">
+        <v>36.981999999999999</v>
+      </c>
+      <c r="AF21">
+        <v>34.280999999999999</v>
+      </c>
+      <c r="AG21">
+        <v>17.123000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22">
+        <v>13</v>
+      </c>
+      <c r="C22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22">
+        <v>183</v>
+      </c>
+      <c r="G22">
+        <v>95</v>
+      </c>
+      <c r="H22">
+        <v>64</v>
+      </c>
+      <c r="I22">
+        <v>85.01</v>
+      </c>
+      <c r="J22">
+        <v>95.68</v>
+      </c>
+      <c r="K22">
+        <v>67.430000000000007</v>
+      </c>
+      <c r="L22">
+        <v>62.15</v>
+      </c>
+      <c r="M22">
+        <v>61.79</v>
+      </c>
+      <c r="N22">
+        <v>40.340000000000003</v>
+      </c>
+      <c r="O22">
+        <v>201.19</v>
+      </c>
+      <c r="P22">
+        <v>23.831</v>
+      </c>
+      <c r="Q22">
+        <v>38.706000000000003</v>
+      </c>
+      <c r="R22">
+        <v>48.01</v>
+      </c>
+      <c r="S22">
+        <v>56.368000000000002</v>
+      </c>
+      <c r="T22">
+        <v>65.123999999999995</v>
+      </c>
+      <c r="U22">
+        <v>70.697000000000003</v>
+      </c>
+      <c r="V22">
+        <v>67.611999999999995</v>
+      </c>
+      <c r="W22">
+        <v>66.069999999999993</v>
+      </c>
+      <c r="X22">
+        <v>48.856000000000002</v>
+      </c>
+      <c r="Y22">
+        <v>56.168999999999997</v>
+      </c>
+      <c r="Z22">
+        <v>72.09</v>
+      </c>
+      <c r="AA22">
+        <v>88.507000000000005</v>
+      </c>
+      <c r="AB22">
+        <v>99.302999999999997</v>
+      </c>
+      <c r="AC22">
+        <v>108.408</v>
+      </c>
+      <c r="AD22">
+        <v>103.73099999999999</v>
+      </c>
+      <c r="AE22">
+        <v>95.671999999999997</v>
+      </c>
+      <c r="AF22">
+        <v>90.149000000000001</v>
+      </c>
+      <c r="AG22">
+        <v>62.984999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23">
+        <v>15</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23">
+        <v>133</v>
+      </c>
+      <c r="G23">
+        <v>84</v>
+      </c>
+      <c r="H23">
+        <v>63</v>
+      </c>
+      <c r="I23">
+        <v>78.989999999999995</v>
+      </c>
+      <c r="J23">
+        <v>77.8</v>
+      </c>
+      <c r="K23">
+        <v>48.14</v>
+      </c>
+      <c r="L23">
+        <v>34</v>
+      </c>
+      <c r="M23">
+        <v>63</v>
+      </c>
+      <c r="N23">
+        <v>21.38</v>
+      </c>
+      <c r="O23">
+        <v>137.31</v>
+      </c>
+      <c r="P23">
+        <v>14.726000000000001</v>
+      </c>
+      <c r="Q23">
+        <v>25.672000000000001</v>
+      </c>
+      <c r="R23">
+        <v>45.97</v>
+      </c>
+      <c r="S23">
+        <v>64.378</v>
+      </c>
+      <c r="T23">
+        <v>68.06</v>
+      </c>
+      <c r="U23">
+        <v>55.622</v>
+      </c>
+      <c r="V23">
+        <v>45.075000000000003</v>
+      </c>
+      <c r="W23">
+        <v>38.209000000000003</v>
+      </c>
+      <c r="X23">
+        <v>33.831000000000003</v>
+      </c>
+      <c r="Y23">
+        <v>33.631999999999998</v>
+      </c>
+      <c r="Z23">
+        <v>47.015000000000001</v>
+      </c>
+      <c r="AA23">
+        <v>67.662000000000006</v>
+      </c>
+      <c r="AB23">
+        <v>77.164000000000001</v>
+      </c>
+      <c r="AC23">
+        <v>82.885999999999996</v>
+      </c>
+      <c r="AD23">
+        <v>87.512</v>
+      </c>
+      <c r="AE23">
+        <v>84.378</v>
+      </c>
+      <c r="AF23">
+        <v>80.846000000000004</v>
+      </c>
+      <c r="AG23">
+        <v>70.745999999999995</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>16</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24">
+        <v>135</v>
+      </c>
+      <c r="G24">
+        <v>84</v>
+      </c>
+      <c r="H24">
+        <v>42</v>
+      </c>
+      <c r="I24">
+        <v>69.930000000000007</v>
+      </c>
+      <c r="J24">
+        <v>83.62</v>
+      </c>
+      <c r="K24">
+        <v>64.42</v>
+      </c>
+      <c r="L24">
+        <v>43.65</v>
+      </c>
+      <c r="M24">
+        <v>41.35</v>
+      </c>
+      <c r="N24">
+        <v>21.59</v>
+      </c>
+      <c r="O24">
+        <v>144.48000000000002</v>
+      </c>
+      <c r="P24">
+        <v>13.881</v>
+      </c>
+      <c r="Q24">
+        <v>22.885999999999999</v>
+      </c>
+      <c r="R24">
+        <v>31.692</v>
+      </c>
+      <c r="S24">
+        <v>42.189</v>
+      </c>
+      <c r="T24">
+        <v>47.761000000000003</v>
+      </c>
+      <c r="U24">
+        <v>46.219000000000001</v>
+      </c>
+      <c r="V24">
+        <v>47.264000000000003</v>
+      </c>
+      <c r="W24">
+        <v>49.055</v>
+      </c>
+      <c r="X24">
+        <v>42.735999999999997</v>
+      </c>
+      <c r="Y24">
+        <v>36.417999999999999</v>
+      </c>
+      <c r="Z24">
+        <v>54.328000000000003</v>
+      </c>
+      <c r="AA24">
+        <v>74.228999999999999</v>
+      </c>
+      <c r="AB24">
+        <v>82.885999999999996</v>
+      </c>
+      <c r="AC24">
+        <v>89.700999999999993</v>
+      </c>
+      <c r="AD24">
+        <v>89.004999999999995</v>
+      </c>
+      <c r="AE24">
+        <v>84.876000000000005</v>
+      </c>
+      <c r="AF24">
+        <v>72.438000000000002</v>
+      </c>
+      <c r="AG24">
+        <v>60.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2">
+        <v>17</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" s="2">
+        <v>167.3</v>
+      </c>
+      <c r="G25" s="2">
+        <v>107.59</v>
+      </c>
+      <c r="H25" s="2">
+        <v>53</v>
+      </c>
+      <c r="I25" s="2">
+        <v>91.75</v>
+      </c>
+      <c r="J25" s="2">
+        <v>96.79</v>
+      </c>
+      <c r="K25" s="2">
+        <v>55.15</v>
+      </c>
+      <c r="L25" s="2">
+        <v>43.49</v>
+      </c>
+      <c r="M25" s="2">
+        <v>45.29</v>
+      </c>
+      <c r="N25" s="2">
+        <v>23.94</v>
+      </c>
+      <c r="O25" s="2">
+        <v>175.82</v>
+      </c>
+      <c r="P25" s="2">
+        <v>18.010000000000002</v>
+      </c>
+      <c r="Q25" s="2">
+        <v>26.219000000000001</v>
+      </c>
+      <c r="R25" s="2">
+        <v>35.372999999999998</v>
+      </c>
+      <c r="S25" s="2">
+        <v>52.438000000000002</v>
+      </c>
+      <c r="T25" s="2">
+        <v>67.412999999999997</v>
+      </c>
+      <c r="U25" s="2">
+        <v>71.343000000000004</v>
+      </c>
+      <c r="V25" s="2">
+        <v>59.005000000000003</v>
+      </c>
+      <c r="W25" s="2">
+        <v>41.741</v>
+      </c>
+      <c r="X25" s="2">
+        <v>28.806000000000001</v>
+      </c>
+      <c r="Y25" s="2">
+        <v>38.557000000000002</v>
+      </c>
+      <c r="Z25" s="2">
+        <v>49.055</v>
+      </c>
+      <c r="AA25" s="2">
+        <v>64.677000000000007</v>
+      </c>
+      <c r="AB25" s="2">
+        <v>82.637</v>
+      </c>
+      <c r="AC25" s="2">
+        <v>100.249</v>
+      </c>
+      <c r="AD25" s="2">
+        <v>109.35299999999999</v>
+      </c>
+      <c r="AE25" s="2">
+        <v>99.501999999999995</v>
+      </c>
+      <c r="AF25" s="2">
+        <v>79.751000000000005</v>
+      </c>
+      <c r="AG25" s="2">
+        <v>38.06</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>57</v>
+      </c>
+      <c r="C26" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26">
+        <v>145</v>
+      </c>
+      <c r="G26">
+        <v>113</v>
+      </c>
+      <c r="H26">
+        <v>51</v>
+      </c>
+      <c r="I26">
+        <v>81.709999999999994</v>
+      </c>
+      <c r="J26">
+        <v>111.07</v>
+      </c>
+      <c r="K26">
+        <v>61.96</v>
+      </c>
+      <c r="L26">
+        <v>36.270000000000003</v>
+      </c>
+      <c r="M26">
+        <v>49.55</v>
+      </c>
+      <c r="N26">
+        <v>30.73</v>
+      </c>
+      <c r="O26">
+        <v>156.37</v>
+      </c>
+      <c r="P26">
+        <v>19.800999999999998</v>
+      </c>
+      <c r="Q26">
+        <v>32.488</v>
+      </c>
+      <c r="R26">
+        <v>45.820999999999998</v>
+      </c>
+      <c r="S26">
+        <v>54.427999999999997</v>
+      </c>
+      <c r="T26">
+        <v>62.536999999999999</v>
+      </c>
+      <c r="U26">
+        <v>60.945</v>
+      </c>
+      <c r="V26">
+        <v>49.850999999999999</v>
+      </c>
+      <c r="W26">
+        <v>38.606999999999999</v>
+      </c>
+      <c r="X26">
+        <v>24.08</v>
+      </c>
+      <c r="Y26">
+        <v>37.761000000000003</v>
+      </c>
+      <c r="Z26">
+        <v>64.228999999999999</v>
+      </c>
+      <c r="AA26">
+        <v>90.1</v>
+      </c>
+      <c r="AB26">
+        <v>103.98</v>
+      </c>
+      <c r="AC26">
+        <v>117.861</v>
+      </c>
+      <c r="AD26">
+        <v>116.21899999999999</v>
+      </c>
+      <c r="AE26">
+        <v>105.473</v>
+      </c>
+      <c r="AF26">
+        <v>78.108999999999995</v>
+      </c>
+      <c r="AG26">
+        <v>52.387999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27">
+        <v>62</v>
+      </c>
+      <c r="C27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27">
+        <v>153.62</v>
+      </c>
+      <c r="G27">
+        <v>109</v>
+      </c>
+      <c r="H27">
+        <v>58</v>
+      </c>
+      <c r="I27">
+        <v>67</v>
+      </c>
+      <c r="J27">
+        <v>101.9</v>
+      </c>
+      <c r="K27">
+        <v>63.94</v>
+      </c>
+      <c r="L27">
+        <v>26.05</v>
+      </c>
+      <c r="M27">
+        <v>48.35</v>
+      </c>
+      <c r="N27">
+        <v>52.42</v>
+      </c>
+      <c r="O27">
+        <v>164.32999999999998</v>
+      </c>
+      <c r="P27">
+        <v>20.298999999999999</v>
+      </c>
+      <c r="Q27">
+        <v>30.547000000000001</v>
+      </c>
+      <c r="R27">
+        <v>39.850999999999999</v>
+      </c>
+      <c r="S27">
+        <v>50.149000000000001</v>
+      </c>
+      <c r="T27">
+        <v>58.308</v>
+      </c>
+      <c r="U27">
+        <v>64.08</v>
+      </c>
+      <c r="V27">
+        <v>65.472999999999999</v>
+      </c>
+      <c r="W27">
+        <v>54.776000000000003</v>
+      </c>
+      <c r="X27">
+        <v>34.725999999999999</v>
+      </c>
+      <c r="Y27">
+        <v>45.671999999999997</v>
+      </c>
+      <c r="Z27">
+        <v>66.617000000000004</v>
+      </c>
+      <c r="AA27">
+        <v>78.457999999999998</v>
+      </c>
+      <c r="AB27">
+        <v>90.697000000000003</v>
+      </c>
+      <c r="AC27">
+        <v>109.55200000000001</v>
+      </c>
+      <c r="AD27">
+        <v>111.194</v>
+      </c>
+      <c r="AE27">
+        <v>84.924999999999997</v>
+      </c>
+      <c r="AF27">
+        <v>59.154000000000003</v>
+      </c>
+      <c r="AG27">
+        <v>32.04</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28">
+        <v>63</v>
+      </c>
+      <c r="C28" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" t="s">
+        <v>51</v>
+      </c>
+      <c r="E28" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28">
+        <v>167</v>
+      </c>
+      <c r="G28">
+        <v>86</v>
+      </c>
+      <c r="H28">
+        <v>47</v>
+      </c>
+      <c r="I28">
+        <v>86</v>
+      </c>
+      <c r="J28">
+        <v>77.38</v>
+      </c>
+      <c r="K28">
+        <v>38.17</v>
+      </c>
+      <c r="L28">
+        <v>33.880000000000003</v>
+      </c>
+      <c r="M28">
+        <v>44.81</v>
+      </c>
+      <c r="N28">
+        <v>30.86</v>
+      </c>
+      <c r="O28">
+        <v>175.87</v>
+      </c>
+      <c r="P28">
+        <v>18.657</v>
+      </c>
+      <c r="Q28">
+        <v>31.193999999999999</v>
+      </c>
+      <c r="R28">
+        <v>39.353000000000002</v>
+      </c>
+      <c r="S28">
+        <v>45.820999999999998</v>
+      </c>
+      <c r="T28">
+        <v>51.890999999999998</v>
+      </c>
+      <c r="U28">
+        <v>54.328000000000003</v>
+      </c>
+      <c r="V28">
+        <v>50.497999999999998</v>
+      </c>
+      <c r="W28">
+        <v>41.143999999999998</v>
+      </c>
+      <c r="X28">
+        <v>28.657</v>
+      </c>
+      <c r="Y28">
+        <v>26.219000000000001</v>
+      </c>
+      <c r="Z28">
+        <v>35.572000000000003</v>
+      </c>
+      <c r="AA28">
+        <v>54.776000000000003</v>
+      </c>
+      <c r="AB28">
+        <v>66.715999999999994</v>
+      </c>
+      <c r="AC28">
+        <v>83.483000000000004</v>
+      </c>
+      <c r="AD28">
+        <v>91.492999999999995</v>
+      </c>
+      <c r="AE28">
+        <v>93.483000000000004</v>
+      </c>
+      <c r="AF28">
+        <v>82.885999999999996</v>
+      </c>
+      <c r="AG28">
+        <v>62.735999999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29">
+        <v>74</v>
+      </c>
+      <c r="C29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" t="s">
+        <v>41</v>
+      </c>
+      <c r="F29">
+        <v>150</v>
+      </c>
+      <c r="G29">
+        <v>90</v>
+      </c>
+      <c r="H29">
+        <v>73</v>
+      </c>
+      <c r="I29">
+        <v>86.88</v>
+      </c>
+      <c r="J29">
+        <v>73.77</v>
+      </c>
+      <c r="K29">
+        <v>44.09</v>
+      </c>
+      <c r="L29">
+        <v>70.150000000000006</v>
+      </c>
+      <c r="M29">
+        <v>57.66</v>
+      </c>
+      <c r="N29">
+        <v>35.18</v>
+      </c>
+      <c r="O29">
+        <v>167.86</v>
+      </c>
+      <c r="P29">
+        <v>20.646999999999998</v>
+      </c>
+      <c r="Q29">
+        <v>31.244</v>
+      </c>
+      <c r="R29">
+        <v>39.103999999999999</v>
+      </c>
+      <c r="S29">
+        <v>45.572000000000003</v>
+      </c>
+      <c r="T29">
+        <v>58.656999999999996</v>
+      </c>
+      <c r="U29">
+        <v>65.322999999999993</v>
+      </c>
+      <c r="V29">
+        <v>70.995000000000005</v>
+      </c>
+      <c r="W29">
+        <v>74.924999999999997</v>
+      </c>
+      <c r="X29">
+        <v>65.671999999999997</v>
+      </c>
+      <c r="Y29">
+        <v>31.99</v>
+      </c>
+      <c r="Z29">
+        <v>41.293999999999997</v>
+      </c>
+      <c r="AA29">
+        <v>56.119</v>
+      </c>
+      <c r="AB29">
+        <v>70.944999999999993</v>
+      </c>
+      <c r="AC29">
+        <v>80.596999999999994</v>
+      </c>
+      <c r="AD29">
+        <v>93.134</v>
+      </c>
+      <c r="AE29">
+        <v>95.870999999999995</v>
+      </c>
+      <c r="AF29">
+        <v>91.691999999999993</v>
+      </c>
+      <c r="AG29">
+        <v>72.686999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30">
+        <v>102</v>
+      </c>
+      <c r="C30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" t="s">
+        <v>42</v>
+      </c>
+      <c r="F30">
+        <v>129</v>
+      </c>
+      <c r="G30">
+        <v>81</v>
+      </c>
+      <c r="H30">
+        <v>46</v>
+      </c>
+      <c r="I30">
+        <v>67.55</v>
+      </c>
+      <c r="J30">
+        <v>79.849999999999994</v>
+      </c>
+      <c r="K30">
+        <v>51.46</v>
+      </c>
+      <c r="L30">
+        <v>28.58</v>
+      </c>
+      <c r="M30">
+        <v>43.38</v>
+      </c>
+      <c r="N30">
+        <v>36.07</v>
+      </c>
+      <c r="O30">
+        <v>135.92000000000002</v>
+      </c>
+      <c r="P30">
+        <v>17.91</v>
+      </c>
+      <c r="Q30">
+        <v>31.591999999999999</v>
+      </c>
+      <c r="R30">
+        <v>39.353000000000002</v>
+      </c>
+      <c r="S30">
+        <v>47.463000000000001</v>
+      </c>
+      <c r="T30">
+        <v>52.387999999999998</v>
+      </c>
+      <c r="U30">
+        <v>51.841000000000001</v>
+      </c>
+      <c r="V30">
+        <v>46.317999999999998</v>
+      </c>
+      <c r="W30">
+        <v>34.776000000000003</v>
+      </c>
+      <c r="X30">
+        <v>19.204000000000001</v>
+      </c>
+      <c r="Y30">
+        <v>20.696999999999999</v>
+      </c>
+      <c r="Z30">
+        <v>38.209000000000003</v>
+      </c>
+      <c r="AA30">
+        <v>66.269000000000005</v>
+      </c>
+      <c r="AB30">
+        <v>76.069999999999993</v>
+      </c>
+      <c r="AC30">
+        <v>80</v>
+      </c>
+      <c r="AD30">
+        <v>75.522000000000006</v>
+      </c>
+      <c r="AE30">
+        <v>73.781000000000006</v>
+      </c>
+      <c r="AF30">
+        <v>66.516999999999996</v>
+      </c>
+      <c r="AG30">
+        <v>53.433</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31">
+        <v>110</v>
+      </c>
+      <c r="C31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F31">
+        <v>119</v>
+      </c>
+      <c r="G31">
+        <v>93</v>
+      </c>
+      <c r="H31">
+        <v>46</v>
+      </c>
+      <c r="I31">
+        <v>93.24</v>
+      </c>
+      <c r="J31">
+        <v>83.59</v>
+      </c>
+      <c r="K31">
+        <v>52.3</v>
+      </c>
+      <c r="L31">
+        <v>45.31</v>
+      </c>
+      <c r="M31">
+        <v>31.4</v>
+      </c>
+      <c r="N31">
+        <v>18.54</v>
+      </c>
+      <c r="O31">
+        <v>124.69</v>
+      </c>
+      <c r="P31">
+        <v>15.111000000000001</v>
+      </c>
+      <c r="Q31">
+        <v>25.382999999999999</v>
+      </c>
+      <c r="R31">
+        <v>33.481000000000002</v>
+      </c>
+      <c r="S31">
+        <v>43.604999999999997</v>
+      </c>
+      <c r="T31">
+        <v>51.16</v>
+      </c>
+      <c r="U31">
+        <v>58.863999999999997</v>
+      </c>
+      <c r="V31">
+        <v>61.728000000000002</v>
+      </c>
+      <c r="W31">
+        <v>50.37</v>
+      </c>
+      <c r="X31">
+        <v>36.148000000000003</v>
+      </c>
+      <c r="Y31">
+        <v>34.469000000000001</v>
+      </c>
+      <c r="Z31">
+        <v>47.654000000000003</v>
+      </c>
+      <c r="AA31">
+        <v>59.357999999999997</v>
+      </c>
+      <c r="AB31">
+        <v>68.988</v>
+      </c>
+      <c r="AC31">
+        <v>88.84</v>
+      </c>
+      <c r="AD31">
+        <v>90.123000000000005</v>
+      </c>
+      <c r="AE31">
+        <v>93.826999999999998</v>
+      </c>
+      <c r="AF31">
+        <v>88.938000000000002</v>
+      </c>
+      <c r="AG31">
+        <v>76.494</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32">
+        <v>113</v>
+      </c>
+      <c r="C32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" t="s">
+        <v>49</v>
+      </c>
+      <c r="F32">
+        <v>126</v>
+      </c>
+      <c r="G32">
+        <v>80.62</v>
+      </c>
+      <c r="H32">
+        <v>42</v>
+      </c>
+      <c r="I32">
+        <v>47</v>
+      </c>
+      <c r="J32">
+        <v>78</v>
+      </c>
+      <c r="K32">
+        <v>48.6</v>
+      </c>
+      <c r="L32">
+        <v>41.22</v>
+      </c>
+      <c r="M32">
+        <v>40.369999999999997</v>
+      </c>
+      <c r="N32">
+        <v>20.329999999999998</v>
+      </c>
+      <c r="O32">
+        <v>136.15</v>
+      </c>
+      <c r="P32">
+        <v>14.37</v>
+      </c>
+      <c r="Q32">
+        <v>24.542999999999999</v>
+      </c>
+      <c r="R32">
+        <v>32.148000000000003</v>
+      </c>
+      <c r="S32">
+        <v>38.518999999999998</v>
+      </c>
+      <c r="T32">
+        <v>44.84</v>
+      </c>
+      <c r="U32">
+        <v>50.963000000000001</v>
+      </c>
+      <c r="V32">
+        <v>55.802</v>
+      </c>
+      <c r="W32">
+        <v>40.295999999999999</v>
+      </c>
+      <c r="X32">
+        <v>23.259</v>
+      </c>
+      <c r="Y32">
+        <v>27.407</v>
+      </c>
+      <c r="Z32">
+        <v>47.061999999999998</v>
+      </c>
+      <c r="AA32">
+        <v>65.284000000000006</v>
+      </c>
+      <c r="AB32">
+        <v>77.234999999999999</v>
+      </c>
+      <c r="AC32">
+        <v>79.555999999999997</v>
+      </c>
+      <c r="AD32">
+        <v>81.135999999999996</v>
+      </c>
+      <c r="AE32">
+        <v>73.234999999999999</v>
+      </c>
+      <c r="AF32">
+        <v>59.357999999999997</v>
+      </c>
+      <c r="AG32">
+        <v>38.024999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33">
+        <v>114</v>
+      </c>
+      <c r="C33" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" t="s">
+        <v>46</v>
+      </c>
+      <c r="E33" t="s">
+        <v>41</v>
+      </c>
+      <c r="F33">
+        <v>115</v>
+      </c>
+      <c r="G33">
+        <v>78</v>
+      </c>
+      <c r="H33">
+        <v>42</v>
+      </c>
+      <c r="I33">
+        <v>73.87</v>
+      </c>
+      <c r="J33">
+        <v>71.33</v>
+      </c>
+      <c r="K33">
+        <v>61.77</v>
+      </c>
+      <c r="L33">
+        <v>50.99</v>
+      </c>
+      <c r="M33">
+        <v>49.98</v>
+      </c>
+      <c r="N33">
+        <v>32.04</v>
+      </c>
+      <c r="O33">
+        <v>119.85</v>
+      </c>
+      <c r="P33">
+        <v>19.012</v>
+      </c>
+      <c r="Q33">
+        <v>36.691000000000003</v>
+      </c>
+      <c r="R33">
+        <v>42.814999999999998</v>
+      </c>
+      <c r="S33">
+        <v>49.728000000000002</v>
+      </c>
+      <c r="T33">
+        <v>50.469000000000001</v>
+      </c>
+      <c r="U33">
+        <v>53.383000000000003</v>
+      </c>
+      <c r="V33">
+        <v>55.16</v>
+      </c>
+      <c r="W33">
+        <v>50.716000000000001</v>
+      </c>
+      <c r="X33">
+        <v>40.840000000000003</v>
+      </c>
+      <c r="Y33">
+        <v>21.283999999999999</v>
+      </c>
+      <c r="Z33">
+        <v>36.840000000000003</v>
+      </c>
+      <c r="AA33">
+        <v>48.542999999999999</v>
+      </c>
+      <c r="AB33">
+        <v>60.098999999999997</v>
+      </c>
+      <c r="AC33">
+        <v>70.962999999999994</v>
+      </c>
+      <c r="AD33">
+        <v>77.382999999999996</v>
+      </c>
+      <c r="AE33">
+        <v>74.221999999999994</v>
+      </c>
+      <c r="AF33">
+        <v>65.284000000000006</v>
+      </c>
+      <c r="AG33">
+        <v>49.877000000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34">
+        <v>115</v>
+      </c>
+      <c r="C34" t="s">
+        <v>43</v>
+      </c>
+      <c r="D34" t="s">
+        <v>44</v>
+      </c>
+      <c r="E34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F34">
+        <v>121</v>
+      </c>
+      <c r="G34">
+        <v>114</v>
+      </c>
+      <c r="H34">
+        <v>50</v>
+      </c>
+      <c r="I34">
+        <v>82.95</v>
+      </c>
+      <c r="J34">
+        <v>99.37</v>
+      </c>
+      <c r="K34">
+        <v>67.2</v>
+      </c>
+      <c r="L34">
+        <v>47.05</v>
+      </c>
+      <c r="M34">
+        <v>44.63</v>
+      </c>
+      <c r="N34">
+        <v>27.15</v>
+      </c>
+      <c r="O34">
+        <v>154.57</v>
+      </c>
+      <c r="P34">
+        <v>12.542999999999999</v>
+      </c>
+      <c r="Q34">
+        <v>22.617000000000001</v>
+      </c>
+      <c r="R34">
+        <v>32.691000000000003</v>
+      </c>
+      <c r="S34">
+        <v>40.542999999999999</v>
+      </c>
+      <c r="T34">
+        <v>48.247</v>
+      </c>
+      <c r="U34">
+        <v>51.704000000000001</v>
+      </c>
+      <c r="V34">
+        <v>52.098999999999997</v>
+      </c>
+      <c r="W34">
+        <v>53.877000000000002</v>
+      </c>
+      <c r="X34">
+        <v>47.259</v>
+      </c>
+      <c r="Y34">
+        <v>35.061999999999998</v>
+      </c>
+      <c r="Z34">
+        <v>63.110999999999997</v>
+      </c>
+      <c r="AA34">
+        <v>77.974999999999994</v>
+      </c>
+      <c r="AB34">
+        <v>97.135999999999996</v>
+      </c>
+      <c r="AC34">
+        <v>99.259</v>
+      </c>
+      <c r="AD34">
+        <v>96.494</v>
+      </c>
+      <c r="AE34">
+        <v>90.715999999999994</v>
+      </c>
+      <c r="AF34">
+        <v>81.480999999999995</v>
+      </c>
+      <c r="AG34">
+        <v>70.765000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35">
+        <v>226</v>
+      </c>
+      <c r="C35" t="s">
+        <v>43</v>
+      </c>
+      <c r="D35" t="s">
+        <v>51</v>
+      </c>
+      <c r="E35" t="s">
+        <v>42</v>
+      </c>
+      <c r="F35">
+        <v>156</v>
+      </c>
+      <c r="G35">
+        <v>106</v>
+      </c>
+      <c r="H35">
+        <v>57</v>
+      </c>
+      <c r="I35">
+        <v>96.86</v>
+      </c>
+      <c r="J35">
+        <v>90.31</v>
+      </c>
+      <c r="K35">
+        <v>50.24</v>
+      </c>
+      <c r="L35">
+        <v>50.41</v>
+      </c>
+      <c r="M35">
+        <v>55</v>
+      </c>
+      <c r="N35">
+        <v>26.4</v>
+      </c>
+      <c r="O35">
+        <v>159.80000000000001</v>
+      </c>
+      <c r="P35">
+        <v>22.934999999999999</v>
+      </c>
+      <c r="Q35">
+        <v>38.408000000000001</v>
+      </c>
+      <c r="R35">
+        <v>50.298999999999999</v>
+      </c>
+      <c r="S35">
+        <v>54.776000000000003</v>
+      </c>
+      <c r="T35">
+        <v>55.97</v>
+      </c>
+      <c r="U35">
+        <v>63.482999999999997</v>
+      </c>
+      <c r="V35">
+        <v>63.93</v>
+      </c>
+      <c r="W35">
+        <v>54.627000000000002</v>
+      </c>
+      <c r="X35">
+        <v>34.527000000000001</v>
+      </c>
+      <c r="Y35">
+        <v>31.890999999999998</v>
+      </c>
+      <c r="Z35">
+        <v>50.646999999999998</v>
+      </c>
+      <c r="AA35">
+        <v>60.198999999999998</v>
+      </c>
+      <c r="AB35">
+        <v>77.611999999999995</v>
+      </c>
+      <c r="AC35">
+        <v>97.91</v>
+      </c>
+      <c r="AD35">
+        <v>102.09</v>
+      </c>
+      <c r="AE35">
+        <v>103.333</v>
+      </c>
+      <c r="AF35">
+        <v>89.9</v>
+      </c>
+      <c r="AG35">
+        <v>48.656999999999996</v>
+      </c>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36">
+        <v>2012</v>
+      </c>
+      <c r="C36" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" t="s">
+        <v>39</v>
+      </c>
+      <c r="E36" t="s">
+        <v>42</v>
+      </c>
+      <c r="F36">
+        <v>174</v>
+      </c>
+      <c r="G36">
+        <v>84</v>
+      </c>
+      <c r="H36">
+        <v>75</v>
+      </c>
+      <c r="I36">
+        <v>67.42</v>
+      </c>
+      <c r="J36">
+        <v>82.58</v>
+      </c>
+      <c r="K36">
+        <v>58.12</v>
+      </c>
+      <c r="L36">
+        <v>34.6</v>
+      </c>
+      <c r="M36">
+        <v>73.569999999999993</v>
+      </c>
+      <c r="N36">
+        <v>51.2</v>
+      </c>
+      <c r="O36">
+        <v>178.90999999999997</v>
+      </c>
+      <c r="P36">
+        <v>18.507000000000001</v>
+      </c>
+      <c r="Q36">
+        <v>36.965000000000003</v>
+      </c>
+      <c r="R36">
+        <v>48.408000000000001</v>
+      </c>
+      <c r="S36">
+        <v>54.776000000000003</v>
+      </c>
+      <c r="T36">
+        <v>75.721000000000004</v>
+      </c>
+      <c r="U36">
+        <v>95.622</v>
+      </c>
+      <c r="V36">
+        <v>82.388000000000005</v>
+      </c>
+      <c r="W36">
+        <v>59.552</v>
+      </c>
+      <c r="X36">
+        <v>39.9</v>
+      </c>
+      <c r="Y36">
+        <v>32.735999999999997</v>
+      </c>
+      <c r="Z36">
+        <v>58.01</v>
+      </c>
+      <c r="AA36">
+        <v>78.108999999999995</v>
+      </c>
+      <c r="AB36">
+        <v>85.174000000000007</v>
+      </c>
+      <c r="AC36">
+        <v>84.179000000000002</v>
+      </c>
+      <c r="AD36">
+        <v>81.244</v>
+      </c>
+      <c r="AE36">
+        <v>70.796000000000006</v>
+      </c>
+      <c r="AF36">
+        <v>58.259</v>
+      </c>
+      <c r="AG36">
+        <v>46.816000000000003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37">
+        <v>2042</v>
+      </c>
+      <c r="C37" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" t="s">
+        <v>51</v>
+      </c>
+      <c r="E37" t="s">
+        <v>42</v>
+      </c>
+      <c r="F37">
+        <v>158</v>
+      </c>
+      <c r="G37">
+        <v>86</v>
+      </c>
+      <c r="H37">
+        <v>60</v>
+      </c>
+      <c r="I37">
+        <v>64.739999999999995</v>
+      </c>
+      <c r="J37">
+        <v>84.12</v>
+      </c>
+      <c r="K37">
+        <v>58.27</v>
+      </c>
+      <c r="L37">
+        <v>39.54</v>
+      </c>
+      <c r="M37">
+        <v>60</v>
+      </c>
+      <c r="N37">
+        <v>25.41</v>
+      </c>
+      <c r="O37">
+        <v>168.46</v>
+      </c>
+      <c r="P37">
+        <v>15.622</v>
+      </c>
+      <c r="Q37">
+        <v>34.328000000000003</v>
+      </c>
+      <c r="R37">
+        <v>58.109000000000002</v>
+      </c>
+      <c r="S37">
+        <v>60.697000000000003</v>
+      </c>
+      <c r="T37">
+        <v>61.692</v>
+      </c>
+      <c r="U37">
+        <v>63.085000000000001</v>
+      </c>
+      <c r="V37">
+        <v>62.786000000000001</v>
+      </c>
+      <c r="W37">
+        <v>53.731000000000002</v>
+      </c>
+      <c r="X37">
+        <v>42.289000000000001</v>
+      </c>
+      <c r="Y37">
+        <v>41.542000000000002</v>
+      </c>
+      <c r="Z37">
+        <v>53.631999999999998</v>
+      </c>
+      <c r="AA37">
+        <v>73.581999999999994</v>
+      </c>
+      <c r="AB37">
+        <v>77.164000000000001</v>
+      </c>
+      <c r="AC37">
+        <v>86.07</v>
+      </c>
+      <c r="AD37">
+        <v>79.004999999999995</v>
+      </c>
+      <c r="AE37">
+        <v>70.596999999999994</v>
+      </c>
+      <c r="AF37">
+        <v>60.398000000000003</v>
+      </c>
+      <c r="AG37">
+        <v>42.488</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{383660EC-002B-4F82-AD45-B527AFD2D4AC}">
+  <dimension ref="A1:AG48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:AG48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T1" t="s">
+        <v>5</v>
+      </c>
+      <c r="U1" t="s">
+        <v>6</v>
+      </c>
+      <c r="V1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2">
+        <v>159</v>
+      </c>
+      <c r="G2">
+        <v>79</v>
+      </c>
+      <c r="H2">
+        <v>78.67</v>
+      </c>
+      <c r="I2">
+        <v>55.7</v>
+      </c>
+      <c r="J2">
+        <v>73.31</v>
+      </c>
+      <c r="K2">
+        <v>43.92</v>
+      </c>
+      <c r="L2">
+        <v>74.64</v>
+      </c>
+      <c r="M2">
+        <v>43.46</v>
+      </c>
+      <c r="N2">
+        <v>22.3</v>
+      </c>
+      <c r="O2">
+        <v>163.95</v>
+      </c>
+      <c r="P2">
+        <v>15.704000000000001</v>
+      </c>
+      <c r="Q2">
+        <v>20.888999999999999</v>
+      </c>
+      <c r="R2">
+        <v>30.765000000000001</v>
+      </c>
+      <c r="S2">
+        <v>36.295999999999999</v>
+      </c>
+      <c r="T2">
+        <v>54.173000000000002</v>
+      </c>
+      <c r="U2">
+        <v>71.209999999999994</v>
+      </c>
+      <c r="V2">
+        <v>75.852000000000004</v>
+      </c>
+      <c r="W2">
+        <v>75.308999999999997</v>
+      </c>
+      <c r="X2">
+        <v>64.346000000000004</v>
+      </c>
+      <c r="Y2">
+        <v>28.741</v>
+      </c>
+      <c r="Z2">
+        <v>42.073999999999998</v>
+      </c>
+      <c r="AA2">
+        <v>59.654000000000003</v>
+      </c>
+      <c r="AB2">
+        <v>73.284000000000006</v>
+      </c>
+      <c r="AC2">
+        <v>77.876999999999995</v>
+      </c>
+      <c r="AD2">
+        <v>76.296000000000006</v>
+      </c>
+      <c r="AE2">
+        <v>64.84</v>
+      </c>
+      <c r="AF2">
+        <v>54.320999999999998</v>
+      </c>
+      <c r="AG2">
+        <v>41.332999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>22</v>
+      </c>
+      <c r="O3">
+        <v>97.23</v>
+      </c>
+      <c r="P3">
+        <v>12.593</v>
+      </c>
+      <c r="Q3">
+        <v>16.84</v>
+      </c>
+      <c r="R3">
+        <v>23.704000000000001</v>
+      </c>
+      <c r="S3">
+        <v>29.777999999999999</v>
+      </c>
+      <c r="T3">
+        <v>35.308999999999997</v>
+      </c>
+      <c r="U3">
+        <v>41.926000000000002</v>
+      </c>
+      <c r="V3">
+        <v>50.37</v>
+      </c>
+      <c r="W3">
+        <v>43.802</v>
+      </c>
+      <c r="X3">
+        <v>24.937999999999999</v>
+      </c>
+      <c r="Y3">
+        <v>14.519</v>
+      </c>
+      <c r="Z3">
+        <v>24.295999999999999</v>
+      </c>
+      <c r="AA3">
+        <v>32.889000000000003</v>
+      </c>
+      <c r="AB3">
+        <v>38.914000000000001</v>
+      </c>
+      <c r="AC3">
+        <v>43.061999999999998</v>
+      </c>
+      <c r="AD3">
+        <v>46.024999999999999</v>
+      </c>
+      <c r="AE3">
+        <v>49.530999999999999</v>
+      </c>
+      <c r="AF3">
+        <v>55.753</v>
+      </c>
+      <c r="AG3">
+        <v>63.259</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4">
         <v>23</v>
       </c>
       <c r="O4">
@@ -1122,7 +4872,7 @@
         <v>57.68</v>
       </c>
     </row>
-    <row r="8" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -1225,7 +4975,7 @@
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9">
         <v>35</v>
@@ -1290,7 +5040,7 @@
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10">
         <v>36</v>
@@ -3457,7 +7207,7 @@
         <v>60.5</v>
       </c>
     </row>
-    <row r="34" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A34" s="2" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
EG10 silhouettes remade and remeasured.
</commit_message>
<xml_diff>
--- a/data/Caliper_ImageJ_comparison.xlsx
+++ b/data/Caliper_ImageJ_comparison.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FilesVC\GMM-exp-boxgrove-gona\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA75792-C606-483E-A238-53E95C0D35A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92BF420D-5BE5-41EC-A8D8-5F0D5BAA4E01}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="52">
   <si>
     <t>site</t>
   </si>
@@ -197,10 +197,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -516,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG37"/>
+  <dimension ref="A1:AG45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1438,7 +1444,7 @@
         <v>21</v>
       </c>
       <c r="B10">
-        <v>1125</v>
+        <v>1121</v>
       </c>
       <c r="C10" t="s">
         <v>38</v>
@@ -1447,91 +1453,91 @@
         <v>47</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F10">
-        <v>85.3</v>
+        <v>79.599999999999994</v>
       </c>
       <c r="G10">
-        <v>65.8</v>
+        <v>43.9</v>
       </c>
       <c r="H10">
-        <v>35</v>
+        <v>42.6</v>
       </c>
       <c r="I10">
-        <v>56.6</v>
+        <v>42.4</v>
       </c>
       <c r="J10">
-        <v>64.900000000000006</v>
+        <v>41.3</v>
       </c>
       <c r="K10">
-        <v>54.1</v>
+        <v>30.4</v>
       </c>
       <c r="L10">
-        <v>26.2</v>
+        <v>33.6</v>
       </c>
       <c r="M10">
-        <v>34.799999999999997</v>
+        <v>38</v>
       </c>
       <c r="N10">
-        <v>24.4</v>
+        <v>25.3</v>
       </c>
       <c r="O10">
-        <v>77.42</v>
+        <v>76.399999999999991</v>
       </c>
       <c r="P10">
-        <v>18.582999999999998</v>
+        <v>13.947000000000001</v>
       </c>
       <c r="Q10">
-        <v>25.75</v>
+        <v>24.210999999999999</v>
       </c>
       <c r="R10">
-        <v>29.542000000000002</v>
+        <v>32.280999999999999</v>
       </c>
       <c r="S10">
-        <v>34.667000000000002</v>
+        <v>36.886000000000003</v>
       </c>
       <c r="T10">
-        <v>37.082999999999998</v>
+        <v>38.946999999999996</v>
       </c>
       <c r="U10">
-        <v>37.707999999999998</v>
+        <v>41.753999999999998</v>
       </c>
       <c r="V10">
-        <v>35.082999999999998</v>
+        <v>42.192999999999998</v>
       </c>
       <c r="W10">
-        <v>31.167000000000002</v>
+        <v>38.246000000000002</v>
       </c>
       <c r="X10">
-        <v>25.792000000000002</v>
+        <v>23.772000000000002</v>
       </c>
       <c r="Y10">
-        <v>34.738999999999997</v>
+        <v>19.561</v>
       </c>
       <c r="Z10">
-        <v>47.042999999999999</v>
+        <v>29.824999999999999</v>
       </c>
       <c r="AA10">
-        <v>61.652000000000001</v>
+        <v>34.210999999999999</v>
       </c>
       <c r="AB10">
-        <v>64.912999999999997</v>
+        <v>37.807000000000002</v>
       </c>
       <c r="AC10">
-        <v>66.260999999999996</v>
+        <v>41.009</v>
       </c>
       <c r="AD10">
-        <v>64.912999999999997</v>
+        <v>43.070000000000007</v>
       </c>
       <c r="AE10">
-        <v>61.87</v>
+        <v>43.158000000000001</v>
       </c>
       <c r="AF10">
-        <v>50.738999999999997</v>
+        <v>40.658000000000001</v>
       </c>
       <c r="AG10">
-        <v>34.783000000000001</v>
+        <v>29.911999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.45">
@@ -1539,100 +1545,100 @@
         <v>21</v>
       </c>
       <c r="B11">
-        <v>1184</v>
-      </c>
-      <c r="C11" t="s">
+        <v>1125</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D11" t="s">
         <v>47</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F11">
-        <v>104.7</v>
+        <v>85.3</v>
       </c>
       <c r="G11">
-        <v>71.400000000000006</v>
+        <v>65.8</v>
       </c>
       <c r="H11">
-        <v>50.8</v>
+        <v>35</v>
       </c>
       <c r="I11">
-        <v>45.7</v>
+        <v>56.6</v>
       </c>
       <c r="J11">
-        <v>67.2</v>
+        <v>64.900000000000006</v>
       </c>
       <c r="K11">
-        <v>38.799999999999997</v>
+        <v>54.1</v>
       </c>
       <c r="L11">
-        <v>38.700000000000003</v>
+        <v>26.2</v>
       </c>
       <c r="M11">
-        <v>48.3</v>
+        <v>34.799999999999997</v>
       </c>
       <c r="N11">
-        <v>41.7</v>
+        <v>24.4</v>
       </c>
       <c r="O11">
-        <v>102.25</v>
+        <v>85.52</v>
       </c>
       <c r="P11">
-        <v>14.628</v>
+        <v>18.583000000000002</v>
       </c>
       <c r="Q11">
-        <v>32.975000000000001</v>
+        <v>25.75</v>
       </c>
       <c r="R11">
-        <v>50.744</v>
+        <v>29.542000000000002</v>
       </c>
       <c r="S11">
-        <v>60.164999999999999</v>
+        <v>34.667000000000002</v>
       </c>
       <c r="T11">
-        <v>63.802</v>
+        <v>37.082999999999998</v>
       </c>
       <c r="U11">
-        <v>60.247999999999998</v>
+        <v>37.707999999999998</v>
       </c>
       <c r="V11">
-        <v>55.124000000000002</v>
+        <v>35.082999999999998</v>
       </c>
       <c r="W11">
-        <v>41.156999999999996</v>
+        <v>31.166999999999998</v>
       </c>
       <c r="X11">
-        <v>24.297999999999998</v>
+        <v>25.792000000000002</v>
       </c>
       <c r="Y11">
-        <v>26.5</v>
+        <v>34.738999999999997</v>
       </c>
       <c r="Z11">
-        <v>39.542000000000002</v>
+        <v>47.042999999999999</v>
       </c>
       <c r="AA11">
-        <v>46.042000000000002</v>
+        <v>61.651999999999994</v>
       </c>
       <c r="AB11">
-        <v>49.707999999999998</v>
+        <v>64.912999999999997</v>
       </c>
       <c r="AC11">
-        <v>52.207999999999998</v>
+        <v>66.260999999999996</v>
       </c>
       <c r="AD11">
-        <v>53.042000000000002</v>
+        <v>64.912999999999997</v>
       </c>
       <c r="AE11">
-        <v>51.5</v>
+        <v>61.870000000000005</v>
       </c>
       <c r="AF11">
-        <v>43.875</v>
+        <v>50.739000000000004</v>
       </c>
       <c r="AG11">
-        <v>27.207999999999998</v>
+        <v>34.783000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.45">
@@ -1640,97 +1646,100 @@
         <v>21</v>
       </c>
       <c r="B12">
-        <v>1223</v>
+        <v>1171</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s">
         <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="F12">
-        <v>82</v>
+        <v>86.3</v>
       </c>
       <c r="G12">
-        <v>57.7</v>
+        <v>61.5</v>
       </c>
       <c r="H12">
-        <v>38.9</v>
+        <v>39.799999999999997</v>
       </c>
       <c r="I12">
-        <v>50.4</v>
+        <v>57.9</v>
       </c>
       <c r="J12">
-        <v>57.1</v>
+        <v>60.1</v>
       </c>
       <c r="K12">
-        <v>48.5</v>
+        <v>27</v>
       </c>
       <c r="L12">
-        <v>26.9</v>
+        <v>30.4</v>
       </c>
       <c r="M12">
-        <v>38.299999999999997</v>
+        <v>34</v>
+      </c>
+      <c r="N12">
+        <v>23</v>
       </c>
       <c r="O12">
-        <v>81.820000000000007</v>
+        <v>78</v>
       </c>
       <c r="P12">
-        <v>12.241</v>
+        <v>16.86</v>
       </c>
       <c r="Q12">
-        <v>20.776</v>
+        <v>24.628</v>
       </c>
       <c r="R12">
-        <v>31.466000000000001</v>
+        <v>26.198</v>
       </c>
       <c r="S12">
-        <v>41.25</v>
+        <v>27.974999999999998</v>
       </c>
       <c r="T12">
-        <v>42.112000000000002</v>
+        <v>28.759999999999998</v>
       </c>
       <c r="U12">
-        <v>42.026000000000003</v>
+        <v>28.759999999999998</v>
       </c>
       <c r="V12">
-        <v>38.146999999999998</v>
+        <v>29.091000000000001</v>
       </c>
       <c r="W12">
-        <v>32.5</v>
+        <v>29.834999999999997</v>
       </c>
       <c r="X12">
-        <v>25.603000000000002</v>
+        <v>26.942</v>
       </c>
       <c r="Y12">
-        <v>26.489000000000001</v>
+        <v>33.091000000000001</v>
       </c>
       <c r="Z12">
-        <v>45.689</v>
+        <v>46.544999999999995</v>
       </c>
       <c r="AA12">
-        <v>51.822000000000003</v>
+        <v>44.908999999999999</v>
       </c>
       <c r="AB12">
-        <v>54.311</v>
+        <v>47.727000000000004</v>
       </c>
       <c r="AC12">
-        <v>55.289000000000001</v>
+        <v>55.909000000000006</v>
       </c>
       <c r="AD12">
-        <v>53.155999999999999</v>
+        <v>52.954999999999998</v>
       </c>
       <c r="AE12">
-        <v>48.844000000000001</v>
+        <v>51.817999999999998</v>
       </c>
       <c r="AF12">
-        <v>43.244</v>
+        <v>44.817999999999998</v>
       </c>
       <c r="AG12">
-        <v>33.421999999999997</v>
+        <v>39.091000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.45">
@@ -1738,7 +1747,7 @@
         <v>21</v>
       </c>
       <c r="B13">
-        <v>1320</v>
+        <v>1184</v>
       </c>
       <c r="C13" t="s">
         <v>38</v>
@@ -1750,88 +1759,88 @@
         <v>49</v>
       </c>
       <c r="F13">
-        <v>81.2</v>
+        <v>104.7</v>
       </c>
       <c r="G13">
-        <v>66.8</v>
+        <v>71.400000000000006</v>
       </c>
       <c r="H13">
-        <v>59.6</v>
+        <v>50.8</v>
       </c>
       <c r="I13">
-        <v>62.8</v>
+        <v>45.7</v>
       </c>
       <c r="J13">
-        <v>65.599999999999994</v>
+        <v>67.2</v>
       </c>
       <c r="K13">
-        <v>50.9</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="L13">
-        <v>57.4</v>
+        <v>38.700000000000003</v>
       </c>
       <c r="M13">
-        <v>59.6</v>
+        <v>48.3</v>
       </c>
       <c r="N13">
-        <v>52.4</v>
+        <v>41.7</v>
       </c>
       <c r="O13">
-        <v>80.55</v>
+        <v>102.25</v>
       </c>
       <c r="P13">
-        <v>40.167000000000002</v>
+        <v>14.628</v>
       </c>
       <c r="Q13">
-        <v>48.536000000000001</v>
+        <v>32.975000000000001</v>
       </c>
       <c r="R13">
-        <v>52.802999999999997</v>
+        <v>50.744</v>
       </c>
       <c r="S13">
-        <v>55.23</v>
+        <v>60.164999999999999</v>
       </c>
       <c r="T13">
-        <v>56.987000000000002</v>
+        <v>63.802000000000007</v>
       </c>
       <c r="U13">
-        <v>55.314</v>
+        <v>60.247999999999998</v>
       </c>
       <c r="V13">
-        <v>52.05</v>
+        <v>55.124000000000002</v>
       </c>
       <c r="W13">
-        <v>48.451999999999998</v>
+        <v>41.157000000000004</v>
       </c>
       <c r="X13">
-        <v>43.472999999999999</v>
+        <v>24.298000000000002</v>
       </c>
       <c r="Y13">
-        <v>27.553000000000001</v>
+        <v>26.5</v>
       </c>
       <c r="Z13">
-        <v>49.494</v>
+        <v>39.542000000000002</v>
       </c>
       <c r="AA13">
-        <v>58.143000000000001</v>
+        <v>46.041999999999994</v>
       </c>
       <c r="AB13">
-        <v>62.743000000000002</v>
+        <v>49.707999999999998</v>
       </c>
       <c r="AC13">
-        <v>67.215000000000003</v>
+        <v>52.207999999999998</v>
       </c>
       <c r="AD13">
-        <v>67.468000000000004</v>
+        <v>53.042000000000002</v>
       </c>
       <c r="AE13">
-        <v>62.658000000000001</v>
+        <v>51.5</v>
       </c>
       <c r="AF13">
-        <v>56.286999999999999</v>
+        <v>43.875</v>
       </c>
       <c r="AG13">
-        <v>42.024999999999999</v>
+        <v>27.208000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.45">
@@ -1839,7 +1848,7 @@
         <v>21</v>
       </c>
       <c r="B14">
-        <v>1559</v>
+        <v>1215</v>
       </c>
       <c r="C14" t="s">
         <v>38</v>
@@ -1851,96 +1860,96 @@
         <v>49</v>
       </c>
       <c r="F14">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G14">
-        <v>56.3</v>
+        <v>53.2</v>
       </c>
       <c r="H14">
-        <v>34.6</v>
+        <v>45.5</v>
       </c>
       <c r="I14">
-        <v>52.1</v>
+        <v>48.4</v>
       </c>
       <c r="J14">
-        <v>49.8</v>
+        <v>51.2</v>
       </c>
       <c r="K14">
-        <v>44.8</v>
+        <v>43.4</v>
       </c>
       <c r="L14">
-        <v>34.4</v>
+        <v>31.9</v>
       </c>
       <c r="M14">
-        <v>34.5</v>
+        <v>45</v>
       </c>
       <c r="N14">
-        <v>33.5</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="O14">
-        <v>78.09</v>
+        <v>76.7</v>
       </c>
       <c r="P14">
-        <v>22.92</v>
+        <v>17.815000000000001</v>
       </c>
       <c r="Q14">
-        <v>30.12</v>
+        <v>30</v>
       </c>
       <c r="R14">
-        <v>33.28</v>
+        <v>38.823999999999998</v>
       </c>
       <c r="S14">
-        <v>33.96</v>
+        <v>44.118000000000002</v>
       </c>
       <c r="T14">
-        <v>34.28</v>
+        <v>45.335999999999999</v>
       </c>
       <c r="U14">
-        <v>34.08</v>
+        <v>43.570999999999998</v>
       </c>
       <c r="V14">
-        <v>33.880000000000003</v>
+        <v>37.563000000000002</v>
       </c>
       <c r="W14">
-        <v>33.880000000000003</v>
+        <v>29.832000000000001</v>
       </c>
       <c r="X14">
-        <v>30.32</v>
+        <v>17.143000000000001</v>
       </c>
       <c r="Y14">
-        <v>24.489000000000001</v>
+        <v>30.739000000000001</v>
       </c>
       <c r="Z14">
-        <v>41.732999999999997</v>
+        <v>42.783000000000001</v>
       </c>
       <c r="AA14">
-        <v>49.2</v>
+        <v>50.609000000000002</v>
       </c>
       <c r="AB14">
-        <v>56.488999999999997</v>
+        <v>53.564999999999998</v>
       </c>
       <c r="AC14">
-        <v>60.267000000000003</v>
+        <v>54</v>
       </c>
       <c r="AD14">
-        <v>59.421999999999997</v>
+        <v>53.826000000000001</v>
       </c>
       <c r="AE14">
-        <v>51.777999999999999</v>
+        <v>52.435000000000002</v>
       </c>
       <c r="AF14">
-        <v>38.889000000000003</v>
+        <v>47.826000000000008</v>
       </c>
       <c r="AG14">
-        <v>23.733000000000001</v>
+        <v>39.216999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15">
-        <v>2002</v>
+        <v>1223</v>
       </c>
       <c r="C15" t="s">
         <v>38</v>
@@ -1949,503 +1958,500 @@
         <v>47</v>
       </c>
       <c r="E15" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="F15">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="G15">
-        <v>38</v>
+        <v>57.7</v>
       </c>
       <c r="H15">
-        <v>32</v>
+        <v>38.9</v>
       </c>
       <c r="I15">
-        <v>35.6</v>
+        <v>50.4</v>
       </c>
       <c r="J15">
-        <v>37.5</v>
+        <v>57.1</v>
       </c>
       <c r="K15">
-        <v>31.6</v>
+        <v>48.5</v>
       </c>
       <c r="L15">
-        <v>26.7</v>
+        <v>26.9</v>
       </c>
       <c r="M15">
-        <v>31</v>
-      </c>
-      <c r="N15">
-        <v>26.9</v>
+        <v>38.299999999999997</v>
       </c>
       <c r="O15">
-        <v>48.16</v>
+        <v>81.820000000000007</v>
       </c>
       <c r="P15">
-        <v>16.706</v>
+        <v>12.241</v>
       </c>
       <c r="Q15">
-        <v>24.869</v>
+        <v>20.776</v>
       </c>
       <c r="R15">
-        <v>28.222000000000001</v>
+        <v>31.465999999999998</v>
       </c>
       <c r="S15">
-        <v>30.728999999999999</v>
+        <v>41.25</v>
       </c>
       <c r="T15">
-        <v>31.137</v>
+        <v>42.111999999999995</v>
       </c>
       <c r="U15">
-        <v>32.156999999999996</v>
+        <v>42.026000000000003</v>
       </c>
       <c r="V15">
-        <v>34.869</v>
+        <v>38.147000000000006</v>
       </c>
       <c r="W15">
-        <v>30.321000000000002</v>
+        <v>32.5</v>
       </c>
       <c r="X15">
-        <v>20.233000000000001</v>
+        <v>25.602999999999998</v>
       </c>
       <c r="Y15">
-        <v>27.318000000000001</v>
+        <v>26.488999999999997</v>
       </c>
       <c r="Z15">
-        <v>31.545000000000002</v>
+        <v>45.689</v>
       </c>
       <c r="AA15">
-        <v>33.293999999999997</v>
+        <v>51.822000000000003</v>
       </c>
       <c r="AB15">
-        <v>36.792999999999999</v>
+        <v>54.311</v>
       </c>
       <c r="AC15">
-        <v>38.570999999999998</v>
+        <v>55.289000000000001</v>
       </c>
       <c r="AD15">
-        <v>37.405000000000001</v>
+        <v>53.155999999999999</v>
       </c>
       <c r="AE15">
-        <v>35.948</v>
+        <v>48.844000000000001</v>
       </c>
       <c r="AF15">
-        <v>34.344000000000001</v>
+        <v>43.244</v>
       </c>
       <c r="AG15">
-        <v>26.617999999999999</v>
+        <v>33.421999999999997</v>
       </c>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16">
-        <v>2006</v>
+        <v>1302</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
         <v>47</v>
       </c>
       <c r="E16" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="F16">
-        <v>42</v>
+        <v>103.9</v>
       </c>
       <c r="G16">
-        <v>34</v>
+        <v>71.599999999999994</v>
       </c>
       <c r="H16">
-        <v>16</v>
+        <v>60.1</v>
       </c>
       <c r="I16">
-        <v>29.8</v>
+        <v>64.2</v>
       </c>
       <c r="J16">
-        <v>31.3</v>
+        <v>70.3</v>
       </c>
       <c r="K16">
-        <v>27.1</v>
+        <v>53.8</v>
       </c>
       <c r="L16">
-        <v>13.9</v>
+        <v>55.1</v>
       </c>
       <c r="M16">
-        <v>15.2</v>
+        <v>60</v>
       </c>
       <c r="N16">
-        <v>13.1</v>
+        <v>40</v>
       </c>
       <c r="O16">
-        <v>43.58</v>
+        <v>104.16</v>
       </c>
       <c r="P16">
-        <v>5.7539999999999996</v>
+        <v>30.535</v>
       </c>
       <c r="Q16">
-        <v>12.316000000000001</v>
+        <v>49.218000000000004</v>
       </c>
       <c r="R16">
-        <v>16.07</v>
+        <v>57.449000000000005</v>
       </c>
       <c r="S16">
-        <v>17.965</v>
+        <v>60.823</v>
       </c>
       <c r="T16">
-        <v>18.315999999999999</v>
+        <v>60.494</v>
       </c>
       <c r="U16">
-        <v>18.105</v>
+        <v>69.63</v>
       </c>
       <c r="V16">
-        <v>17.684000000000001</v>
+        <v>64.938000000000002</v>
       </c>
       <c r="W16">
-        <v>16.07</v>
+        <v>54.402999999999999</v>
       </c>
       <c r="X16">
-        <v>12.175000000000001</v>
+        <v>39.259</v>
       </c>
       <c r="Y16">
-        <v>23.509</v>
+        <v>44.28</v>
       </c>
       <c r="Z16">
-        <v>28.911999999999999</v>
+        <v>51.111000000000004</v>
       </c>
       <c r="AA16">
-        <v>30.596</v>
+        <v>65.513999999999996</v>
       </c>
       <c r="AB16">
-        <v>33.228000000000002</v>
+        <v>70.494</v>
       </c>
       <c r="AC16">
-        <v>32.350999999999999</v>
+        <v>72.387</v>
       </c>
       <c r="AD16">
-        <v>31.123000000000001</v>
+        <v>69.341999999999999</v>
       </c>
       <c r="AE16">
-        <v>29.439</v>
+        <v>64.198000000000008</v>
       </c>
       <c r="AF16">
-        <v>27.367999999999999</v>
+        <v>54.896999999999998</v>
       </c>
       <c r="AG16">
-        <v>25.544</v>
+        <v>37.86</v>
       </c>
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17">
-        <v>2016</v>
+        <v>1320</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
         <v>47</v>
       </c>
       <c r="E17" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="F17">
-        <v>73</v>
+        <v>81.2</v>
       </c>
       <c r="G17">
-        <v>49</v>
+        <v>66.8</v>
       </c>
       <c r="H17">
-        <v>46</v>
+        <v>59.6</v>
       </c>
       <c r="I17">
-        <v>41.3</v>
+        <v>62.8</v>
       </c>
       <c r="J17">
-        <v>41.6</v>
+        <v>65.599999999999994</v>
       </c>
       <c r="K17">
-        <v>28.3</v>
+        <v>50.9</v>
       </c>
       <c r="L17">
-        <v>14.7</v>
+        <v>57.4</v>
       </c>
       <c r="M17">
-        <v>25</v>
+        <v>59.6</v>
       </c>
       <c r="N17">
-        <v>14.2</v>
+        <v>52.4</v>
       </c>
       <c r="O17">
-        <v>79.710000000000008</v>
+        <v>80.55</v>
       </c>
       <c r="P17">
-        <v>14.84</v>
+        <v>40.167000000000002</v>
       </c>
       <c r="Q17">
-        <v>21.37</v>
+        <v>48.536000000000001</v>
       </c>
       <c r="R17">
-        <v>27.725999999999999</v>
+        <v>52.803000000000004</v>
       </c>
       <c r="S17">
-        <v>32.478000000000002</v>
+        <v>55.23</v>
       </c>
       <c r="T17">
-        <v>37.872</v>
+        <v>56.986999999999995</v>
       </c>
       <c r="U17">
-        <v>44.402000000000001</v>
+        <v>55.313999999999993</v>
       </c>
       <c r="V17">
-        <v>48.892000000000003</v>
+        <v>52.05</v>
       </c>
       <c r="W17">
-        <v>51.223999999999997</v>
+        <v>48.451999999999998</v>
       </c>
       <c r="X17">
-        <v>44.636000000000003</v>
+        <v>43.472999999999999</v>
       </c>
       <c r="Y17">
-        <v>20.350000000000001</v>
+        <v>27.553000000000001</v>
       </c>
       <c r="Z17">
-        <v>27.492999999999999</v>
+        <v>49.494</v>
       </c>
       <c r="AA17">
-        <v>32.594999999999999</v>
+        <v>58.143000000000001</v>
       </c>
       <c r="AB17">
-        <v>38.250999999999998</v>
+        <v>62.743000000000002</v>
       </c>
       <c r="AC17">
-        <v>48.192</v>
+        <v>67.215000000000003</v>
       </c>
       <c r="AD17">
-        <v>53.12</v>
+        <v>67.468000000000004</v>
       </c>
       <c r="AE17">
-        <v>52.012</v>
+        <v>62.657999999999994</v>
       </c>
       <c r="AF17">
-        <v>50.146000000000001</v>
+        <v>56.287000000000006</v>
       </c>
       <c r="AG17">
-        <v>38.22</v>
+        <v>42.024999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18">
-        <v>2066</v>
+        <v>1334</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D18" t="s">
         <v>47</v>
       </c>
       <c r="E18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F18">
-        <v>44</v>
+        <v>85.1</v>
       </c>
       <c r="G18">
-        <v>33</v>
+        <v>50.6</v>
       </c>
       <c r="H18">
-        <v>27</v>
+        <v>44.4</v>
       </c>
       <c r="I18">
-        <v>29.8</v>
+        <v>49.1</v>
       </c>
       <c r="J18">
-        <v>28.3</v>
+        <v>47.9</v>
       </c>
       <c r="K18">
-        <v>19.399999999999999</v>
+        <v>34.6</v>
       </c>
       <c r="L18">
-        <v>25.2</v>
+        <v>42.8</v>
       </c>
       <c r="M18">
-        <v>25.4</v>
+        <v>44.1</v>
       </c>
       <c r="N18">
-        <v>19.600000000000001</v>
+        <v>35.6</v>
       </c>
       <c r="O18">
-        <v>45.129999999999995</v>
+        <v>84.3</v>
       </c>
       <c r="P18">
-        <v>11.603</v>
+        <v>25.390999999999998</v>
       </c>
       <c r="Q18">
-        <v>15.16</v>
+        <v>35.652000000000001</v>
       </c>
       <c r="R18">
-        <v>18.251000000000001</v>
+        <v>40.174000000000007</v>
       </c>
       <c r="S18">
-        <v>22.187000000000001</v>
+        <v>43.913000000000004</v>
       </c>
       <c r="T18">
-        <v>25.044</v>
+        <v>48.521999999999998</v>
       </c>
       <c r="U18">
-        <v>28.28</v>
+        <v>46.826000000000001</v>
       </c>
       <c r="V18">
-        <v>31.195</v>
+        <v>42.173999999999992</v>
       </c>
       <c r="W18">
-        <v>33.090000000000003</v>
+        <v>35.739000000000004</v>
       </c>
       <c r="X18">
-        <v>32.186999999999998</v>
+        <v>17.826000000000001</v>
       </c>
       <c r="Y18">
-        <v>12.65</v>
+        <v>12.565</v>
       </c>
       <c r="Z18">
-        <v>18.076000000000001</v>
+        <v>27.216999999999999</v>
       </c>
       <c r="AA18">
-        <v>19.649999999999999</v>
+        <v>43.87</v>
       </c>
       <c r="AB18">
-        <v>20</v>
+        <v>48.738999999999997</v>
       </c>
       <c r="AC18">
-        <v>23.994</v>
+        <v>50.521999999999998</v>
       </c>
       <c r="AD18">
-        <v>27.93</v>
+        <v>49.783000000000001</v>
       </c>
       <c r="AE18">
-        <v>29.738</v>
+        <v>50.260999999999996</v>
       </c>
       <c r="AF18">
-        <v>30.117000000000001</v>
+        <v>42.695999999999998</v>
       </c>
       <c r="AG18">
-        <v>25.19</v>
+        <v>22.347999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19">
-        <v>2081</v>
+        <v>1335</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D19" t="s">
         <v>47</v>
       </c>
       <c r="E19" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="F19">
-        <v>47</v>
+        <v>68.2</v>
       </c>
       <c r="G19">
-        <v>38</v>
+        <v>55.7</v>
       </c>
       <c r="H19">
-        <v>25</v>
+        <v>33.200000000000003</v>
       </c>
       <c r="I19">
-        <v>37.5</v>
+        <v>49.9</v>
       </c>
       <c r="J19">
-        <v>34.200000000000003</v>
+        <v>53.1</v>
       </c>
       <c r="K19">
-        <v>23.8</v>
+        <v>33.200000000000003</v>
       </c>
       <c r="L19">
-        <v>25.4</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="M19">
-        <v>23.3</v>
+        <v>33</v>
       </c>
       <c r="N19">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="O19">
-        <v>44.960000000000008</v>
+        <v>67.430000000000007</v>
       </c>
       <c r="P19">
-        <v>15.218999999999999</v>
+        <v>17.190000000000001</v>
       </c>
       <c r="Q19">
-        <v>19.359000000000002</v>
+        <v>27.850999999999999</v>
       </c>
       <c r="R19">
-        <v>22.710999999999999</v>
+        <v>35.908999999999999</v>
       </c>
       <c r="S19">
-        <v>27.143000000000001</v>
+        <v>40.660999999999994</v>
       </c>
       <c r="T19">
-        <v>29.3</v>
+        <v>41.280999999999999</v>
       </c>
       <c r="U19">
-        <v>29.853999999999999</v>
+        <v>37.850999999999999</v>
       </c>
       <c r="V19">
-        <v>28.192</v>
+        <v>35.868000000000002</v>
       </c>
       <c r="W19">
-        <v>24.547999999999998</v>
+        <v>29.007999999999999</v>
       </c>
       <c r="X19">
-        <v>16.268000000000001</v>
+        <v>20.825999999999997</v>
       </c>
       <c r="Y19">
-        <v>22.157</v>
+        <v>24.247999999999998</v>
       </c>
       <c r="Z19">
-        <v>31.777999999999999</v>
+        <v>34.69</v>
       </c>
       <c r="AA19">
-        <v>33.527999999999999</v>
+        <v>42.565999999999995</v>
       </c>
       <c r="AB19">
-        <v>34.14</v>
+        <v>48.761000000000003</v>
       </c>
       <c r="AC19">
-        <v>35.889000000000003</v>
+        <v>54.292000000000002</v>
       </c>
       <c r="AD19">
-        <v>37.637999999999998</v>
+        <v>54.158999999999999</v>
       </c>
       <c r="AE19">
-        <v>39.095999999999997</v>
+        <v>48.141999999999996</v>
       </c>
       <c r="AF19">
-        <v>36.064</v>
+        <v>38.673000000000002</v>
       </c>
       <c r="AG19">
-        <v>29.5</v>
+        <v>26.46</v>
       </c>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20">
-        <v>2092</v>
+        <v>1533</v>
       </c>
       <c r="C20" t="s">
         <v>38</v>
@@ -2454,1000 +2460,1000 @@
         <v>47</v>
       </c>
       <c r="E20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F20">
-        <v>41</v>
+        <v>80.400000000000006</v>
       </c>
       <c r="G20">
-        <v>33.1</v>
+        <v>56</v>
       </c>
       <c r="H20">
-        <v>26</v>
+        <v>56.8</v>
       </c>
       <c r="I20">
-        <v>24.3</v>
+        <v>48.3</v>
       </c>
       <c r="J20">
-        <v>31.3</v>
+        <v>47</v>
       </c>
       <c r="K20">
-        <v>21.3</v>
+        <v>36.700000000000003</v>
       </c>
       <c r="L20">
-        <v>22</v>
+        <v>36.5</v>
       </c>
       <c r="M20">
-        <v>24.7</v>
+        <v>49.6</v>
       </c>
       <c r="N20">
-        <v>22</v>
+        <v>25.8</v>
       </c>
       <c r="O20">
+        <v>77.78</v>
+      </c>
+      <c r="P20">
+        <v>28.291</v>
+      </c>
+      <c r="Q20">
+        <v>35.298999999999999</v>
+      </c>
+      <c r="R20">
+        <v>39.230999999999995</v>
+      </c>
+      <c r="S20">
         <v>42.35</v>
       </c>
-      <c r="P20">
-        <v>15.474</v>
-      </c>
-      <c r="Q20">
-        <v>21.228000000000002</v>
-      </c>
-      <c r="R20">
-        <v>25.93</v>
-      </c>
-      <c r="S20">
-        <v>27.719000000000001</v>
-      </c>
       <c r="T20">
-        <v>27.332999999999998</v>
+        <v>42.777999999999999</v>
       </c>
       <c r="U20">
-        <v>27.367999999999999</v>
+        <v>42.521000000000001</v>
       </c>
       <c r="V20">
-        <v>27.544</v>
+        <v>40.811999999999998</v>
       </c>
       <c r="W20">
-        <v>26.946999999999999</v>
+        <v>41.538000000000004</v>
       </c>
       <c r="X20">
-        <v>26.105</v>
+        <v>32.564</v>
       </c>
       <c r="Y20">
-        <v>16.175000000000001</v>
+        <v>36.838000000000001</v>
       </c>
       <c r="Z20">
-        <v>20.876999999999999</v>
+        <v>43.59</v>
       </c>
       <c r="AA20">
-        <v>25.719000000000001</v>
+        <v>52.137</v>
       </c>
       <c r="AB20">
-        <v>29.053000000000001</v>
+        <v>51.281999999999996</v>
       </c>
       <c r="AC20">
-        <v>30.491</v>
+        <v>47.265000000000001</v>
       </c>
       <c r="AD20">
-        <v>29.193000000000001</v>
+        <v>41.795000000000002</v>
       </c>
       <c r="AE20">
-        <v>28.210999999999999</v>
+        <v>37.265000000000001</v>
       </c>
       <c r="AF20">
-        <v>26.667000000000002</v>
+        <v>30.512999999999998</v>
       </c>
       <c r="AG20">
-        <v>20.526</v>
+        <v>13.419</v>
       </c>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21">
-        <v>2114</v>
-      </c>
-      <c r="C21" t="s">
+        <v>1545</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D21" t="s">
         <v>47</v>
       </c>
       <c r="E21" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="F21">
-        <v>49</v>
+        <v>84.5</v>
       </c>
       <c r="G21">
-        <v>39</v>
+        <v>68.400000000000006</v>
       </c>
       <c r="H21">
-        <v>38</v>
+        <v>66.099999999999994</v>
       </c>
       <c r="I21">
-        <v>37.700000000000003</v>
+        <v>65.400000000000006</v>
       </c>
       <c r="J21">
-        <v>30.9</v>
+        <v>66.5</v>
       </c>
       <c r="K21">
-        <v>27.7</v>
+        <v>57.6</v>
       </c>
       <c r="L21">
-        <v>30.4</v>
+        <v>51.8</v>
       </c>
       <c r="M21">
-        <v>34.200000000000003</v>
+        <v>63</v>
       </c>
       <c r="N21">
-        <v>21.3</v>
+        <v>42.4</v>
       </c>
       <c r="O21">
-        <v>50.25</v>
+        <v>81.53</v>
       </c>
       <c r="P21">
-        <v>16.491</v>
+        <v>27.332999999999998</v>
       </c>
       <c r="Q21">
-        <v>22.315999999999999</v>
+        <v>39.582999999999998</v>
       </c>
       <c r="R21">
-        <v>26.876999999999999</v>
+        <v>51</v>
       </c>
       <c r="S21">
-        <v>30.946999999999999</v>
+        <v>61.25</v>
       </c>
       <c r="T21">
-        <v>34.737000000000002</v>
+        <v>65.625</v>
       </c>
       <c r="U21">
-        <v>35.543999999999997</v>
+        <v>62.582999999999998</v>
       </c>
       <c r="V21">
-        <v>35.683999999999997</v>
+        <v>55.833000000000006</v>
       </c>
       <c r="W21">
-        <v>34.174999999999997</v>
+        <v>47.417000000000002</v>
       </c>
       <c r="X21">
-        <v>33.789000000000001</v>
+        <v>34.25</v>
       </c>
       <c r="Y21">
-        <v>12.420999999999999</v>
+        <v>43.387999999999998</v>
       </c>
       <c r="Z21">
-        <v>26.280999999999999</v>
+        <v>51.942000000000007</v>
       </c>
       <c r="AA21">
-        <v>29.614000000000001</v>
+        <v>57.478999999999999</v>
       </c>
       <c r="AB21">
-        <v>31.053000000000001</v>
+        <v>62.230999999999995</v>
       </c>
       <c r="AC21">
-        <v>35.332999999999998</v>
+        <v>65.579000000000008</v>
       </c>
       <c r="AD21">
-        <v>40.316000000000003</v>
+        <v>66.488</v>
       </c>
       <c r="AE21">
-        <v>36.981999999999999</v>
+        <v>67.230999999999995</v>
       </c>
       <c r="AF21">
-        <v>34.280999999999999</v>
+        <v>64.710999999999999</v>
       </c>
       <c r="AG21">
-        <v>17.123000000000001</v>
+        <v>54.463000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B22">
-        <v>13</v>
+        <v>1559</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D22" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E22" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="F22">
-        <v>183</v>
+        <v>80</v>
       </c>
       <c r="G22">
-        <v>95</v>
+        <v>56.3</v>
       </c>
       <c r="H22">
-        <v>64</v>
+        <v>34.6</v>
       </c>
       <c r="I22">
-        <v>85.01</v>
+        <v>52.1</v>
       </c>
       <c r="J22">
-        <v>95.68</v>
+        <v>49.8</v>
       </c>
       <c r="K22">
-        <v>67.430000000000007</v>
+        <v>44.8</v>
       </c>
       <c r="L22">
-        <v>62.15</v>
+        <v>34.4</v>
       </c>
       <c r="M22">
-        <v>61.79</v>
+        <v>34.5</v>
       </c>
       <c r="N22">
-        <v>40.340000000000003</v>
+        <v>33.5</v>
       </c>
       <c r="O22">
-        <v>201.19</v>
+        <v>78.09</v>
       </c>
       <c r="P22">
-        <v>23.831</v>
+        <v>33.332999999999998</v>
       </c>
       <c r="Q22">
-        <v>38.706000000000003</v>
+        <v>36.267000000000003</v>
       </c>
       <c r="R22">
-        <v>48.01</v>
+        <v>36.356000000000002</v>
       </c>
       <c r="S22">
-        <v>56.368000000000002</v>
+        <v>35.555999999999997</v>
       </c>
       <c r="T22">
-        <v>65.123999999999995</v>
+        <v>35.466999999999999</v>
       </c>
       <c r="U22">
-        <v>70.697000000000003</v>
+        <v>35.200000000000003</v>
       </c>
       <c r="V22">
-        <v>67.611999999999995</v>
+        <v>34.933</v>
       </c>
       <c r="W22">
-        <v>66.069999999999993</v>
+        <v>34.667000000000002</v>
       </c>
       <c r="X22">
-        <v>48.856000000000002</v>
+        <v>29.422000000000001</v>
       </c>
       <c r="Y22">
-        <v>56.168999999999997</v>
+        <v>24.489000000000001</v>
       </c>
       <c r="Z22">
-        <v>72.09</v>
+        <v>41.733000000000004</v>
       </c>
       <c r="AA22">
-        <v>88.507000000000005</v>
+        <v>49.2</v>
       </c>
       <c r="AB22">
-        <v>99.302999999999997</v>
+        <v>56.489000000000004</v>
       </c>
       <c r="AC22">
-        <v>108.408</v>
+        <v>60.266999999999996</v>
       </c>
       <c r="AD22">
-        <v>103.73099999999999</v>
+        <v>59.421999999999997</v>
       </c>
       <c r="AE22">
-        <v>95.671999999999997</v>
+        <v>51.778000000000006</v>
       </c>
       <c r="AF22">
-        <v>90.149000000000001</v>
+        <v>38.889000000000003</v>
       </c>
       <c r="AG22">
-        <v>62.984999999999999</v>
+        <v>23.733000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B23">
-        <v>15</v>
+        <v>2002</v>
       </c>
       <c r="C23" t="s">
         <v>38</v>
       </c>
       <c r="D23" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F23">
-        <v>133</v>
+        <v>46</v>
       </c>
       <c r="G23">
-        <v>84</v>
+        <v>38</v>
       </c>
       <c r="H23">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="I23">
-        <v>78.989999999999995</v>
+        <v>35.6</v>
       </c>
       <c r="J23">
-        <v>77.8</v>
+        <v>37.5</v>
       </c>
       <c r="K23">
-        <v>48.14</v>
+        <v>31.6</v>
       </c>
       <c r="L23">
-        <v>34</v>
+        <v>26.7</v>
       </c>
       <c r="M23">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="N23">
-        <v>21.38</v>
+        <v>26.9</v>
       </c>
       <c r="O23">
-        <v>137.31</v>
+        <v>48.16</v>
       </c>
       <c r="P23">
-        <v>14.726000000000001</v>
+        <v>16.706</v>
       </c>
       <c r="Q23">
-        <v>25.672000000000001</v>
+        <v>24.869</v>
       </c>
       <c r="R23">
-        <v>45.97</v>
+        <v>28.222000000000001</v>
       </c>
       <c r="S23">
-        <v>64.378</v>
+        <v>30.728999999999999</v>
       </c>
       <c r="T23">
-        <v>68.06</v>
+        <v>31.137</v>
       </c>
       <c r="U23">
-        <v>55.622</v>
+        <v>32.156999999999996</v>
       </c>
       <c r="V23">
-        <v>45.075000000000003</v>
+        <v>34.869</v>
       </c>
       <c r="W23">
-        <v>38.209000000000003</v>
+        <v>30.321000000000002</v>
       </c>
       <c r="X23">
-        <v>33.831000000000003</v>
+        <v>20.233000000000001</v>
       </c>
       <c r="Y23">
-        <v>33.631999999999998</v>
+        <v>27.318000000000001</v>
       </c>
       <c r="Z23">
-        <v>47.015000000000001</v>
+        <v>31.545000000000002</v>
       </c>
       <c r="AA23">
-        <v>67.662000000000006</v>
+        <v>33.293999999999997</v>
       </c>
       <c r="AB23">
-        <v>77.164000000000001</v>
+        <v>36.792999999999999</v>
       </c>
       <c r="AC23">
-        <v>82.885999999999996</v>
+        <v>38.570999999999998</v>
       </c>
       <c r="AD23">
-        <v>87.512</v>
+        <v>37.405000000000001</v>
       </c>
       <c r="AE23">
-        <v>84.378</v>
+        <v>35.948</v>
       </c>
       <c r="AF23">
-        <v>80.846000000000004</v>
+        <v>34.344000000000001</v>
       </c>
       <c r="AG23">
-        <v>70.745999999999995</v>
+        <v>26.617999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>16</v>
+        <v>2006</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D24" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E24" t="s">
         <v>42</v>
       </c>
       <c r="F24">
-        <v>135</v>
+        <v>42</v>
       </c>
       <c r="G24">
-        <v>84</v>
+        <v>34</v>
       </c>
       <c r="H24">
+        <v>16</v>
+      </c>
+      <c r="I24">
+        <v>29.8</v>
+      </c>
+      <c r="J24">
+        <v>31.3</v>
+      </c>
+      <c r="K24">
+        <v>27.1</v>
+      </c>
+      <c r="L24">
+        <v>13.9</v>
+      </c>
+      <c r="M24">
+        <v>15.2</v>
+      </c>
+      <c r="N24">
+        <v>13.1</v>
+      </c>
+      <c r="O24">
+        <v>43.58</v>
+      </c>
+      <c r="P24">
+        <v>5.7539999999999996</v>
+      </c>
+      <c r="Q24">
+        <v>12.316000000000001</v>
+      </c>
+      <c r="R24">
+        <v>16.07</v>
+      </c>
+      <c r="S24">
+        <v>17.965</v>
+      </c>
+      <c r="T24">
+        <v>18.315999999999999</v>
+      </c>
+      <c r="U24">
+        <v>18.105</v>
+      </c>
+      <c r="V24">
+        <v>17.684000000000001</v>
+      </c>
+      <c r="W24">
+        <v>16.07</v>
+      </c>
+      <c r="X24">
+        <v>12.175000000000001</v>
+      </c>
+      <c r="Y24">
+        <v>23.509</v>
+      </c>
+      <c r="Z24">
+        <v>28.911999999999999</v>
+      </c>
+      <c r="AA24">
+        <v>30.596</v>
+      </c>
+      <c r="AB24">
+        <v>33.228000000000002</v>
+      </c>
+      <c r="AC24">
+        <v>32.350999999999999</v>
+      </c>
+      <c r="AD24">
+        <v>31.123000000000001</v>
+      </c>
+      <c r="AE24">
+        <v>29.439</v>
+      </c>
+      <c r="AF24">
+        <v>27.367999999999999</v>
+      </c>
+      <c r="AG24">
+        <v>25.544</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25">
+        <v>2016</v>
+      </c>
+      <c r="C25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" t="s">
         <v>42</v>
       </c>
-      <c r="I24">
-        <v>69.930000000000007</v>
-      </c>
-      <c r="J24">
-        <v>83.62</v>
-      </c>
-      <c r="K24">
-        <v>64.42</v>
-      </c>
-      <c r="L24">
-        <v>43.65</v>
-      </c>
-      <c r="M24">
-        <v>41.35</v>
-      </c>
-      <c r="N24">
-        <v>21.59</v>
-      </c>
-      <c r="O24">
-        <v>144.48000000000002</v>
-      </c>
-      <c r="P24">
-        <v>13.881</v>
-      </c>
-      <c r="Q24">
-        <v>22.885999999999999</v>
-      </c>
-      <c r="R24">
-        <v>31.692</v>
-      </c>
-      <c r="S24">
-        <v>42.189</v>
-      </c>
-      <c r="T24">
-        <v>47.761000000000003</v>
-      </c>
-      <c r="U24">
-        <v>46.219000000000001</v>
-      </c>
-      <c r="V24">
-        <v>47.264000000000003</v>
-      </c>
-      <c r="W24">
-        <v>49.055</v>
-      </c>
-      <c r="X24">
-        <v>42.735999999999997</v>
-      </c>
-      <c r="Y24">
-        <v>36.417999999999999</v>
-      </c>
-      <c r="Z24">
-        <v>54.328000000000003</v>
-      </c>
-      <c r="AA24">
-        <v>74.228999999999999</v>
-      </c>
-      <c r="AB24">
-        <v>82.885999999999996</v>
-      </c>
-      <c r="AC24">
-        <v>89.700999999999993</v>
-      </c>
-      <c r="AD24">
-        <v>89.004999999999995</v>
-      </c>
-      <c r="AE24">
-        <v>84.876000000000005</v>
-      </c>
-      <c r="AF24">
-        <v>72.438000000000002</v>
-      </c>
-      <c r="AG24">
-        <v>60.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="2">
-        <v>17</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F25" s="2">
-        <v>167.3</v>
-      </c>
-      <c r="G25" s="2">
-        <v>107.59</v>
-      </c>
-      <c r="H25" s="2">
-        <v>53</v>
-      </c>
-      <c r="I25" s="2">
-        <v>91.75</v>
-      </c>
-      <c r="J25" s="2">
-        <v>96.79</v>
-      </c>
-      <c r="K25" s="2">
-        <v>55.15</v>
-      </c>
-      <c r="L25" s="2">
-        <v>43.49</v>
-      </c>
-      <c r="M25" s="2">
-        <v>45.29</v>
-      </c>
-      <c r="N25" s="2">
-        <v>23.94</v>
-      </c>
-      <c r="O25" s="2">
-        <v>175.82</v>
-      </c>
-      <c r="P25" s="2">
-        <v>18.010000000000002</v>
-      </c>
-      <c r="Q25" s="2">
-        <v>26.219000000000001</v>
-      </c>
-      <c r="R25" s="2">
-        <v>35.372999999999998</v>
-      </c>
-      <c r="S25" s="2">
-        <v>52.438000000000002</v>
-      </c>
-      <c r="T25" s="2">
-        <v>67.412999999999997</v>
-      </c>
-      <c r="U25" s="2">
-        <v>71.343000000000004</v>
-      </c>
-      <c r="V25" s="2">
-        <v>59.005000000000003</v>
-      </c>
-      <c r="W25" s="2">
-        <v>41.741</v>
-      </c>
-      <c r="X25" s="2">
-        <v>28.806000000000001</v>
-      </c>
-      <c r="Y25" s="2">
-        <v>38.557000000000002</v>
-      </c>
-      <c r="Z25" s="2">
-        <v>49.055</v>
-      </c>
-      <c r="AA25" s="2">
-        <v>64.677000000000007</v>
-      </c>
-      <c r="AB25" s="2">
-        <v>82.637</v>
-      </c>
-      <c r="AC25" s="2">
-        <v>100.249</v>
-      </c>
-      <c r="AD25" s="2">
-        <v>109.35299999999999</v>
-      </c>
-      <c r="AE25" s="2">
-        <v>99.501999999999995</v>
-      </c>
-      <c r="AF25" s="2">
-        <v>79.751000000000005</v>
-      </c>
-      <c r="AG25" s="2">
-        <v>38.06</v>
+      <c r="F25">
+        <v>73</v>
+      </c>
+      <c r="G25">
+        <v>49</v>
+      </c>
+      <c r="H25">
+        <v>46</v>
+      </c>
+      <c r="I25">
+        <v>41.3</v>
+      </c>
+      <c r="J25">
+        <v>41.6</v>
+      </c>
+      <c r="K25">
+        <v>28.3</v>
+      </c>
+      <c r="L25">
+        <v>14.7</v>
+      </c>
+      <c r="M25">
+        <v>25</v>
+      </c>
+      <c r="N25">
+        <v>14.2</v>
+      </c>
+      <c r="O25">
+        <v>79.710000000000008</v>
+      </c>
+      <c r="P25">
+        <v>14.84</v>
+      </c>
+      <c r="Q25">
+        <v>21.37</v>
+      </c>
+      <c r="R25">
+        <v>27.725999999999999</v>
+      </c>
+      <c r="S25">
+        <v>32.478000000000002</v>
+      </c>
+      <c r="T25">
+        <v>37.872</v>
+      </c>
+      <c r="U25">
+        <v>44.402000000000001</v>
+      </c>
+      <c r="V25">
+        <v>48.892000000000003</v>
+      </c>
+      <c r="W25">
+        <v>51.223999999999997</v>
+      </c>
+      <c r="X25">
+        <v>44.636000000000003</v>
+      </c>
+      <c r="Y25">
+        <v>20.350000000000001</v>
+      </c>
+      <c r="Z25">
+        <v>27.492999999999999</v>
+      </c>
+      <c r="AA25">
+        <v>32.594999999999999</v>
+      </c>
+      <c r="AB25">
+        <v>38.250999999999998</v>
+      </c>
+      <c r="AC25">
+        <v>48.192</v>
+      </c>
+      <c r="AD25">
+        <v>53.12</v>
+      </c>
+      <c r="AE25">
+        <v>52.012</v>
+      </c>
+      <c r="AF25">
+        <v>50.146000000000001</v>
+      </c>
+      <c r="AG25">
+        <v>38.22</v>
       </c>
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B26">
-        <v>57</v>
+        <v>2066</v>
       </c>
       <c r="C26" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D26" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E26" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F26">
-        <v>145</v>
+        <v>44</v>
       </c>
       <c r="G26">
-        <v>113</v>
+        <v>33</v>
       </c>
       <c r="H26">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="I26">
-        <v>81.709999999999994</v>
+        <v>29.8</v>
       </c>
       <c r="J26">
-        <v>111.07</v>
+        <v>28.3</v>
       </c>
       <c r="K26">
-        <v>61.96</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="L26">
-        <v>36.270000000000003</v>
+        <v>25.2</v>
       </c>
       <c r="M26">
-        <v>49.55</v>
+        <v>25.4</v>
       </c>
       <c r="N26">
-        <v>30.73</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="O26">
-        <v>156.37</v>
+        <v>45.129999999999995</v>
       </c>
       <c r="P26">
-        <v>19.800999999999998</v>
+        <v>11.603</v>
       </c>
       <c r="Q26">
-        <v>32.488</v>
+        <v>15.16</v>
       </c>
       <c r="R26">
-        <v>45.820999999999998</v>
+        <v>18.251000000000001</v>
       </c>
       <c r="S26">
-        <v>54.427999999999997</v>
+        <v>22.187000000000001</v>
       </c>
       <c r="T26">
-        <v>62.536999999999999</v>
+        <v>25.044</v>
       </c>
       <c r="U26">
-        <v>60.945</v>
+        <v>28.28</v>
       </c>
       <c r="V26">
-        <v>49.850999999999999</v>
+        <v>31.195</v>
       </c>
       <c r="W26">
-        <v>38.606999999999999</v>
+        <v>33.090000000000003</v>
       </c>
       <c r="X26">
-        <v>24.08</v>
+        <v>32.186999999999998</v>
       </c>
       <c r="Y26">
-        <v>37.761000000000003</v>
+        <v>12.65</v>
       </c>
       <c r="Z26">
-        <v>64.228999999999999</v>
+        <v>18.076000000000001</v>
       </c>
       <c r="AA26">
-        <v>90.1</v>
+        <v>19.649999999999999</v>
       </c>
       <c r="AB26">
-        <v>103.98</v>
+        <v>20</v>
       </c>
       <c r="AC26">
-        <v>117.861</v>
+        <v>23.994</v>
       </c>
       <c r="AD26">
-        <v>116.21899999999999</v>
+        <v>27.93</v>
       </c>
       <c r="AE26">
-        <v>105.473</v>
+        <v>29.738</v>
       </c>
       <c r="AF26">
-        <v>78.108999999999995</v>
+        <v>30.117000000000001</v>
       </c>
       <c r="AG26">
-        <v>52.387999999999998</v>
+        <v>25.19</v>
       </c>
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B27">
-        <v>62</v>
+        <v>2081</v>
       </c>
       <c r="C27" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D27" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E27" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F27">
-        <v>153.62</v>
+        <v>47</v>
       </c>
       <c r="G27">
-        <v>109</v>
+        <v>38</v>
       </c>
       <c r="H27">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="I27">
-        <v>67</v>
+        <v>37.5</v>
       </c>
       <c r="J27">
-        <v>101.9</v>
+        <v>34.200000000000003</v>
       </c>
       <c r="K27">
-        <v>63.94</v>
+        <v>23.8</v>
       </c>
       <c r="L27">
-        <v>26.05</v>
+        <v>25.4</v>
       </c>
       <c r="M27">
-        <v>48.35</v>
+        <v>23.3</v>
       </c>
       <c r="N27">
-        <v>52.42</v>
+        <v>18</v>
       </c>
       <c r="O27">
-        <v>164.32999999999998</v>
+        <v>44.960000000000008</v>
       </c>
       <c r="P27">
-        <v>20.298999999999999</v>
+        <v>15.218999999999999</v>
       </c>
       <c r="Q27">
-        <v>30.547000000000001</v>
+        <v>19.359000000000002</v>
       </c>
       <c r="R27">
-        <v>39.850999999999999</v>
+        <v>22.710999999999999</v>
       </c>
       <c r="S27">
-        <v>50.149000000000001</v>
+        <v>27.143000000000001</v>
       </c>
       <c r="T27">
-        <v>58.308</v>
+        <v>29.3</v>
       </c>
       <c r="U27">
-        <v>64.08</v>
+        <v>29.853999999999999</v>
       </c>
       <c r="V27">
-        <v>65.472999999999999</v>
+        <v>28.192</v>
       </c>
       <c r="W27">
-        <v>54.776000000000003</v>
+        <v>24.547999999999998</v>
       </c>
       <c r="X27">
-        <v>34.725999999999999</v>
+        <v>16.268000000000001</v>
       </c>
       <c r="Y27">
-        <v>45.671999999999997</v>
+        <v>22.157</v>
       </c>
       <c r="Z27">
-        <v>66.617000000000004</v>
+        <v>31.777999999999999</v>
       </c>
       <c r="AA27">
-        <v>78.457999999999998</v>
+        <v>33.527999999999999</v>
       </c>
       <c r="AB27">
-        <v>90.697000000000003</v>
+        <v>34.14</v>
       </c>
       <c r="AC27">
-        <v>109.55200000000001</v>
+        <v>35.889000000000003</v>
       </c>
       <c r="AD27">
-        <v>111.194</v>
+        <v>37.637999999999998</v>
       </c>
       <c r="AE27">
-        <v>84.924999999999997</v>
+        <v>39.095999999999997</v>
       </c>
       <c r="AF27">
-        <v>59.154000000000003</v>
+        <v>36.064</v>
       </c>
       <c r="AG27">
-        <v>32.04</v>
+        <v>29.5</v>
       </c>
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B28">
-        <v>63</v>
+        <v>2092</v>
       </c>
       <c r="C28" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D28" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E28" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F28">
-        <v>167</v>
+        <v>41</v>
       </c>
       <c r="G28">
-        <v>86</v>
+        <v>33.1</v>
       </c>
       <c r="H28">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="I28">
-        <v>86</v>
+        <v>24.3</v>
       </c>
       <c r="J28">
-        <v>77.38</v>
+        <v>31.3</v>
       </c>
       <c r="K28">
-        <v>38.17</v>
+        <v>21.3</v>
       </c>
       <c r="L28">
-        <v>33.880000000000003</v>
+        <v>22</v>
       </c>
       <c r="M28">
-        <v>44.81</v>
+        <v>24.7</v>
       </c>
       <c r="N28">
-        <v>30.86</v>
+        <v>22</v>
       </c>
       <c r="O28">
-        <v>175.87</v>
+        <v>42.35</v>
       </c>
       <c r="P28">
-        <v>18.657</v>
+        <v>15.474</v>
       </c>
       <c r="Q28">
-        <v>31.193999999999999</v>
+        <v>21.228000000000002</v>
       </c>
       <c r="R28">
-        <v>39.353000000000002</v>
+        <v>25.93</v>
       </c>
       <c r="S28">
-        <v>45.820999999999998</v>
+        <v>27.719000000000001</v>
       </c>
       <c r="T28">
-        <v>51.890999999999998</v>
+        <v>27.332999999999998</v>
       </c>
       <c r="U28">
-        <v>54.328000000000003</v>
+        <v>27.367999999999999</v>
       </c>
       <c r="V28">
-        <v>50.497999999999998</v>
+        <v>27.544</v>
       </c>
       <c r="W28">
-        <v>41.143999999999998</v>
+        <v>26.946999999999999</v>
       </c>
       <c r="X28">
-        <v>28.657</v>
+        <v>26.105</v>
       </c>
       <c r="Y28">
-        <v>26.219000000000001</v>
+        <v>16.175000000000001</v>
       </c>
       <c r="Z28">
-        <v>35.572000000000003</v>
+        <v>20.876999999999999</v>
       </c>
       <c r="AA28">
-        <v>54.776000000000003</v>
+        <v>25.719000000000001</v>
       </c>
       <c r="AB28">
-        <v>66.715999999999994</v>
+        <v>29.053000000000001</v>
       </c>
       <c r="AC28">
-        <v>83.483000000000004</v>
+        <v>30.491</v>
       </c>
       <c r="AD28">
-        <v>91.492999999999995</v>
+        <v>29.193000000000001</v>
       </c>
       <c r="AE28">
-        <v>93.483000000000004</v>
+        <v>28.210999999999999</v>
       </c>
       <c r="AF28">
-        <v>82.885999999999996</v>
+        <v>26.667000000000002</v>
       </c>
       <c r="AG28">
-        <v>62.735999999999997</v>
+        <v>20.526</v>
       </c>
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B29">
-        <v>74</v>
+        <v>2114</v>
       </c>
       <c r="C29" t="s">
         <v>38</v>
       </c>
       <c r="D29" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E29" t="s">
         <v>41</v>
       </c>
       <c r="F29">
-        <v>150</v>
+        <v>49</v>
       </c>
       <c r="G29">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="H29">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="I29">
-        <v>86.88</v>
+        <v>37.700000000000003</v>
       </c>
       <c r="J29">
-        <v>73.77</v>
+        <v>30.9</v>
       </c>
       <c r="K29">
-        <v>44.09</v>
+        <v>27.7</v>
       </c>
       <c r="L29">
-        <v>70.150000000000006</v>
+        <v>30.4</v>
       </c>
       <c r="M29">
-        <v>57.66</v>
+        <v>34.200000000000003</v>
       </c>
       <c r="N29">
-        <v>35.18</v>
+        <v>21.3</v>
       </c>
       <c r="O29">
-        <v>167.86</v>
+        <v>50.25</v>
       </c>
       <c r="P29">
-        <v>20.646999999999998</v>
+        <v>16.491</v>
       </c>
       <c r="Q29">
-        <v>31.244</v>
+        <v>22.315999999999999</v>
       </c>
       <c r="R29">
-        <v>39.103999999999999</v>
+        <v>26.876999999999999</v>
       </c>
       <c r="S29">
-        <v>45.572000000000003</v>
+        <v>30.946999999999999</v>
       </c>
       <c r="T29">
-        <v>58.656999999999996</v>
+        <v>34.737000000000002</v>
       </c>
       <c r="U29">
-        <v>65.322999999999993</v>
+        <v>35.543999999999997</v>
       </c>
       <c r="V29">
-        <v>70.995000000000005</v>
+        <v>35.683999999999997</v>
       </c>
       <c r="W29">
-        <v>74.924999999999997</v>
+        <v>34.174999999999997</v>
       </c>
       <c r="X29">
-        <v>65.671999999999997</v>
+        <v>33.789000000000001</v>
       </c>
       <c r="Y29">
-        <v>31.99</v>
+        <v>12.420999999999999</v>
       </c>
       <c r="Z29">
-        <v>41.293999999999997</v>
+        <v>26.280999999999999</v>
       </c>
       <c r="AA29">
-        <v>56.119</v>
+        <v>29.614000000000001</v>
       </c>
       <c r="AB29">
-        <v>70.944999999999993</v>
+        <v>31.053000000000001</v>
       </c>
       <c r="AC29">
-        <v>80.596999999999994</v>
+        <v>35.332999999999998</v>
       </c>
       <c r="AD29">
-        <v>93.134</v>
+        <v>40.316000000000003</v>
       </c>
       <c r="AE29">
-        <v>95.870999999999995</v>
+        <v>36.981999999999999</v>
       </c>
       <c r="AF29">
-        <v>91.691999999999993</v>
+        <v>34.280999999999999</v>
       </c>
       <c r="AG29">
-        <v>72.686999999999998</v>
+        <v>17.123000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.45">
@@ -3455,7 +3461,7 @@
         <v>24</v>
       </c>
       <c r="B30">
-        <v>102</v>
+        <v>13</v>
       </c>
       <c r="C30" t="s">
         <v>43</v>
@@ -3467,88 +3473,88 @@
         <v>42</v>
       </c>
       <c r="F30">
-        <v>129</v>
+        <v>183</v>
       </c>
       <c r="G30">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="H30">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="I30">
-        <v>67.55</v>
+        <v>85.01</v>
       </c>
       <c r="J30">
-        <v>79.849999999999994</v>
+        <v>95.68</v>
       </c>
       <c r="K30">
-        <v>51.46</v>
+        <v>67.430000000000007</v>
       </c>
       <c r="L30">
-        <v>28.58</v>
+        <v>62.15</v>
       </c>
       <c r="M30">
-        <v>43.38</v>
+        <v>61.79</v>
       </c>
       <c r="N30">
-        <v>36.07</v>
+        <v>40.340000000000003</v>
       </c>
       <c r="O30">
-        <v>135.92000000000002</v>
+        <v>201.19</v>
       </c>
       <c r="P30">
-        <v>17.91</v>
+        <v>23.831</v>
       </c>
       <c r="Q30">
-        <v>31.591999999999999</v>
+        <v>38.706000000000003</v>
       </c>
       <c r="R30">
-        <v>39.353000000000002</v>
+        <v>48.01</v>
       </c>
       <c r="S30">
-        <v>47.463000000000001</v>
+        <v>56.368000000000002</v>
       </c>
       <c r="T30">
-        <v>52.387999999999998</v>
+        <v>65.123999999999995</v>
       </c>
       <c r="U30">
-        <v>51.841000000000001</v>
+        <v>70.697000000000003</v>
       </c>
       <c r="V30">
-        <v>46.317999999999998</v>
+        <v>67.611999999999995</v>
       </c>
       <c r="W30">
-        <v>34.776000000000003</v>
+        <v>66.069999999999993</v>
       </c>
       <c r="X30">
-        <v>19.204000000000001</v>
+        <v>48.856000000000002</v>
       </c>
       <c r="Y30">
-        <v>20.696999999999999</v>
+        <v>56.168999999999997</v>
       </c>
       <c r="Z30">
-        <v>38.209000000000003</v>
+        <v>72.09</v>
       </c>
       <c r="AA30">
-        <v>66.269000000000005</v>
+        <v>88.507000000000005</v>
       </c>
       <c r="AB30">
-        <v>76.069999999999993</v>
+        <v>99.302999999999997</v>
       </c>
       <c r="AC30">
-        <v>80</v>
+        <v>108.408</v>
       </c>
       <c r="AD30">
-        <v>75.522000000000006</v>
+        <v>103.73099999999999</v>
       </c>
       <c r="AE30">
-        <v>73.781000000000006</v>
+        <v>95.671999999999997</v>
       </c>
       <c r="AF30">
-        <v>66.516999999999996</v>
+        <v>90.149000000000001</v>
       </c>
       <c r="AG30">
-        <v>53.433</v>
+        <v>62.984999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.45">
@@ -3556,100 +3562,100 @@
         <v>24</v>
       </c>
       <c r="B31">
-        <v>110</v>
+        <v>15</v>
       </c>
       <c r="C31" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D31" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E31" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F31">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="G31">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="H31">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="I31">
-        <v>93.24</v>
+        <v>78.989999999999995</v>
       </c>
       <c r="J31">
-        <v>83.59</v>
+        <v>77.8</v>
       </c>
       <c r="K31">
-        <v>52.3</v>
+        <v>48.14</v>
       </c>
       <c r="L31">
-        <v>45.31</v>
+        <v>34</v>
       </c>
       <c r="M31">
-        <v>31.4</v>
+        <v>63</v>
       </c>
       <c r="N31">
-        <v>18.54</v>
+        <v>21.38</v>
       </c>
       <c r="O31">
-        <v>124.69</v>
+        <v>137.31</v>
       </c>
       <c r="P31">
-        <v>15.111000000000001</v>
+        <v>14.726000000000001</v>
       </c>
       <c r="Q31">
-        <v>25.382999999999999</v>
+        <v>25.672000000000001</v>
       </c>
       <c r="R31">
-        <v>33.481000000000002</v>
+        <v>45.97</v>
       </c>
       <c r="S31">
-        <v>43.604999999999997</v>
+        <v>64.378</v>
       </c>
       <c r="T31">
-        <v>51.16</v>
+        <v>68.06</v>
       </c>
       <c r="U31">
-        <v>58.863999999999997</v>
+        <v>55.622</v>
       </c>
       <c r="V31">
-        <v>61.728000000000002</v>
+        <v>45.075000000000003</v>
       </c>
       <c r="W31">
-        <v>50.37</v>
+        <v>38.209000000000003</v>
       </c>
       <c r="X31">
-        <v>36.148000000000003</v>
+        <v>33.831000000000003</v>
       </c>
       <c r="Y31">
-        <v>34.469000000000001</v>
+        <v>33.631999999999998</v>
       </c>
       <c r="Z31">
-        <v>47.654000000000003</v>
+        <v>47.015000000000001</v>
       </c>
       <c r="AA31">
-        <v>59.357999999999997</v>
+        <v>67.662000000000006</v>
       </c>
       <c r="AB31">
-        <v>68.988</v>
+        <v>77.164000000000001</v>
       </c>
       <c r="AC31">
-        <v>88.84</v>
+        <v>82.885999999999996</v>
       </c>
       <c r="AD31">
-        <v>90.123000000000005</v>
+        <v>87.512</v>
       </c>
       <c r="AE31">
-        <v>93.826999999999998</v>
+        <v>84.378</v>
       </c>
       <c r="AF31">
-        <v>88.938000000000002</v>
+        <v>80.846000000000004</v>
       </c>
       <c r="AG31">
-        <v>76.494</v>
+        <v>70.745999999999995</v>
       </c>
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.45">
@@ -3657,201 +3663,201 @@
         <v>24</v>
       </c>
       <c r="B32">
-        <v>113</v>
+        <v>16</v>
       </c>
       <c r="C32" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D32" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E32" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="F32">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="G32">
-        <v>80.62</v>
+        <v>84</v>
       </c>
       <c r="H32">
         <v>42</v>
       </c>
       <c r="I32">
-        <v>47</v>
+        <v>69.930000000000007</v>
       </c>
       <c r="J32">
-        <v>78</v>
+        <v>83.62</v>
       </c>
       <c r="K32">
-        <v>48.6</v>
+        <v>64.42</v>
       </c>
       <c r="L32">
-        <v>41.22</v>
+        <v>43.65</v>
       </c>
       <c r="M32">
-        <v>40.369999999999997</v>
+        <v>41.35</v>
       </c>
       <c r="N32">
-        <v>20.329999999999998</v>
+        <v>21.59</v>
       </c>
       <c r="O32">
-        <v>136.15</v>
+        <v>144.48000000000002</v>
       </c>
       <c r="P32">
-        <v>14.37</v>
+        <v>13.881</v>
       </c>
       <c r="Q32">
-        <v>24.542999999999999</v>
+        <v>22.885999999999999</v>
       </c>
       <c r="R32">
-        <v>32.148000000000003</v>
+        <v>31.692</v>
       </c>
       <c r="S32">
-        <v>38.518999999999998</v>
+        <v>42.189</v>
       </c>
       <c r="T32">
-        <v>44.84</v>
+        <v>47.761000000000003</v>
       </c>
       <c r="U32">
-        <v>50.963000000000001</v>
+        <v>46.219000000000001</v>
       </c>
       <c r="V32">
-        <v>55.802</v>
+        <v>47.264000000000003</v>
       </c>
       <c r="W32">
-        <v>40.295999999999999</v>
+        <v>49.055</v>
       </c>
       <c r="X32">
-        <v>23.259</v>
+        <v>42.735999999999997</v>
       </c>
       <c r="Y32">
-        <v>27.407</v>
+        <v>36.417999999999999</v>
       </c>
       <c r="Z32">
-        <v>47.061999999999998</v>
+        <v>54.328000000000003</v>
       </c>
       <c r="AA32">
-        <v>65.284000000000006</v>
+        <v>74.228999999999999</v>
       </c>
       <c r="AB32">
-        <v>77.234999999999999</v>
+        <v>82.885999999999996</v>
       </c>
       <c r="AC32">
-        <v>79.555999999999997</v>
+        <v>89.700999999999993</v>
       </c>
       <c r="AD32">
-        <v>81.135999999999996</v>
+        <v>89.004999999999995</v>
       </c>
       <c r="AE32">
-        <v>73.234999999999999</v>
+        <v>84.876000000000005</v>
       </c>
       <c r="AF32">
-        <v>59.357999999999997</v>
+        <v>72.438000000000002</v>
       </c>
       <c r="AG32">
-        <v>38.024999999999999</v>
+        <v>60.5</v>
       </c>
     </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
+    <row r="33" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B33">
-        <v>114</v>
-      </c>
-      <c r="C33" t="s">
-        <v>38</v>
-      </c>
-      <c r="D33" t="s">
-        <v>46</v>
-      </c>
-      <c r="E33" t="s">
-        <v>41</v>
-      </c>
-      <c r="F33">
-        <v>115</v>
-      </c>
-      <c r="G33">
-        <v>78</v>
-      </c>
-      <c r="H33">
-        <v>42</v>
-      </c>
-      <c r="I33">
-        <v>73.87</v>
-      </c>
-      <c r="J33">
-        <v>71.33</v>
-      </c>
-      <c r="K33">
-        <v>61.77</v>
-      </c>
-      <c r="L33">
-        <v>50.99</v>
-      </c>
-      <c r="M33">
-        <v>49.98</v>
-      </c>
-      <c r="N33">
-        <v>32.04</v>
-      </c>
-      <c r="O33">
-        <v>119.85</v>
-      </c>
-      <c r="P33">
-        <v>19.012</v>
-      </c>
-      <c r="Q33">
-        <v>36.691000000000003</v>
-      </c>
-      <c r="R33">
-        <v>42.814999999999998</v>
-      </c>
-      <c r="S33">
-        <v>49.728000000000002</v>
-      </c>
-      <c r="T33">
-        <v>50.469000000000001</v>
-      </c>
-      <c r="U33">
-        <v>53.383000000000003</v>
-      </c>
-      <c r="V33">
-        <v>55.16</v>
-      </c>
-      <c r="W33">
-        <v>50.716000000000001</v>
-      </c>
-      <c r="X33">
-        <v>40.840000000000003</v>
-      </c>
-      <c r="Y33">
-        <v>21.283999999999999</v>
-      </c>
-      <c r="Z33">
-        <v>36.840000000000003</v>
-      </c>
-      <c r="AA33">
-        <v>48.542999999999999</v>
-      </c>
-      <c r="AB33">
-        <v>60.098999999999997</v>
-      </c>
-      <c r="AC33">
-        <v>70.962999999999994</v>
-      </c>
-      <c r="AD33">
-        <v>77.382999999999996</v>
-      </c>
-      <c r="AE33">
-        <v>74.221999999999994</v>
-      </c>
-      <c r="AF33">
-        <v>65.284000000000006</v>
-      </c>
-      <c r="AG33">
-        <v>49.877000000000002</v>
+      <c r="B33" s="2">
+        <v>17</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F33" s="2">
+        <v>167.3</v>
+      </c>
+      <c r="G33" s="2">
+        <v>107.59</v>
+      </c>
+      <c r="H33" s="2">
+        <v>53</v>
+      </c>
+      <c r="I33" s="2">
+        <v>91.75</v>
+      </c>
+      <c r="J33" s="2">
+        <v>96.79</v>
+      </c>
+      <c r="K33" s="2">
+        <v>55.15</v>
+      </c>
+      <c r="L33" s="2">
+        <v>43.49</v>
+      </c>
+      <c r="M33" s="2">
+        <v>45.29</v>
+      </c>
+      <c r="N33" s="2">
+        <v>23.94</v>
+      </c>
+      <c r="O33" s="2">
+        <v>175.82</v>
+      </c>
+      <c r="P33" s="2">
+        <v>18.010000000000002</v>
+      </c>
+      <c r="Q33" s="2">
+        <v>26.219000000000001</v>
+      </c>
+      <c r="R33" s="2">
+        <v>35.372999999999998</v>
+      </c>
+      <c r="S33" s="2">
+        <v>52.438000000000002</v>
+      </c>
+      <c r="T33" s="2">
+        <v>67.412999999999997</v>
+      </c>
+      <c r="U33" s="2">
+        <v>71.343000000000004</v>
+      </c>
+      <c r="V33" s="2">
+        <v>59.005000000000003</v>
+      </c>
+      <c r="W33" s="2">
+        <v>41.741</v>
+      </c>
+      <c r="X33" s="2">
+        <v>28.806000000000001</v>
+      </c>
+      <c r="Y33" s="2">
+        <v>38.557000000000002</v>
+      </c>
+      <c r="Z33" s="2">
+        <v>49.055</v>
+      </c>
+      <c r="AA33" s="2">
+        <v>64.677000000000007</v>
+      </c>
+      <c r="AB33" s="2">
+        <v>82.637</v>
+      </c>
+      <c r="AC33" s="2">
+        <v>100.249</v>
+      </c>
+      <c r="AD33" s="2">
+        <v>109.35299999999999</v>
+      </c>
+      <c r="AE33" s="2">
+        <v>99.501999999999995</v>
+      </c>
+      <c r="AF33" s="2">
+        <v>79.751000000000005</v>
+      </c>
+      <c r="AG33" s="2">
+        <v>38.06</v>
       </c>
     </row>
     <row r="34" spans="1:33" x14ac:dyDescent="0.45">
@@ -3859,100 +3865,100 @@
         <v>24</v>
       </c>
       <c r="B34">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="C34" t="s">
         <v>43</v>
       </c>
       <c r="D34" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E34" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="F34">
-        <v>121</v>
+        <v>145</v>
       </c>
       <c r="G34">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H34">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I34">
-        <v>82.95</v>
+        <v>81.709999999999994</v>
       </c>
       <c r="J34">
-        <v>99.37</v>
+        <v>111.07</v>
       </c>
       <c r="K34">
-        <v>67.2</v>
+        <v>61.96</v>
       </c>
       <c r="L34">
-        <v>47.05</v>
+        <v>36.270000000000003</v>
       </c>
       <c r="M34">
-        <v>44.63</v>
+        <v>49.55</v>
       </c>
       <c r="N34">
-        <v>27.15</v>
+        <v>30.73</v>
       </c>
       <c r="O34">
-        <v>154.57</v>
+        <v>156.37</v>
       </c>
       <c r="P34">
-        <v>12.542999999999999</v>
+        <v>19.800999999999998</v>
       </c>
       <c r="Q34">
-        <v>22.617000000000001</v>
+        <v>32.488</v>
       </c>
       <c r="R34">
-        <v>32.691000000000003</v>
+        <v>45.820999999999998</v>
       </c>
       <c r="S34">
-        <v>40.542999999999999</v>
+        <v>54.427999999999997</v>
       </c>
       <c r="T34">
-        <v>48.247</v>
+        <v>62.536999999999999</v>
       </c>
       <c r="U34">
-        <v>51.704000000000001</v>
+        <v>60.945</v>
       </c>
       <c r="V34">
-        <v>52.098999999999997</v>
+        <v>49.850999999999999</v>
       </c>
       <c r="W34">
-        <v>53.877000000000002</v>
+        <v>38.606999999999999</v>
       </c>
       <c r="X34">
-        <v>47.259</v>
+        <v>24.08</v>
       </c>
       <c r="Y34">
-        <v>35.061999999999998</v>
+        <v>37.761000000000003</v>
       </c>
       <c r="Z34">
-        <v>63.110999999999997</v>
+        <v>64.228999999999999</v>
       </c>
       <c r="AA34">
-        <v>77.974999999999994</v>
+        <v>90.1</v>
       </c>
       <c r="AB34">
-        <v>97.135999999999996</v>
+        <v>103.98</v>
       </c>
       <c r="AC34">
-        <v>99.259</v>
+        <v>117.861</v>
       </c>
       <c r="AD34">
-        <v>96.494</v>
+        <v>116.21899999999999</v>
       </c>
       <c r="AE34">
-        <v>90.715999999999994</v>
+        <v>105.473</v>
       </c>
       <c r="AF34">
-        <v>81.480999999999995</v>
+        <v>78.108999999999995</v>
       </c>
       <c r="AG34">
-        <v>70.765000000000001</v>
+        <v>52.387999999999998</v>
       </c>
     </row>
     <row r="35" spans="1:33" x14ac:dyDescent="0.45">
@@ -3960,100 +3966,100 @@
         <v>24</v>
       </c>
       <c r="B35">
-        <v>226</v>
+        <v>62</v>
       </c>
       <c r="C35" t="s">
         <v>43</v>
       </c>
       <c r="D35" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E35" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F35">
-        <v>156</v>
+        <v>153.62</v>
       </c>
       <c r="G35">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="H35">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I35">
-        <v>96.86</v>
+        <v>67</v>
       </c>
       <c r="J35">
-        <v>90.31</v>
+        <v>101.9</v>
       </c>
       <c r="K35">
-        <v>50.24</v>
+        <v>63.94</v>
       </c>
       <c r="L35">
-        <v>50.41</v>
+        <v>26.05</v>
       </c>
       <c r="M35">
-        <v>55</v>
+        <v>48.35</v>
       </c>
       <c r="N35">
-        <v>26.4</v>
+        <v>52.42</v>
       </c>
       <c r="O35">
-        <v>159.80000000000001</v>
+        <v>164.32999999999998</v>
       </c>
       <c r="P35">
-        <v>22.934999999999999</v>
+        <v>20.298999999999999</v>
       </c>
       <c r="Q35">
-        <v>38.408000000000001</v>
+        <v>30.547000000000001</v>
       </c>
       <c r="R35">
-        <v>50.298999999999999</v>
+        <v>39.850999999999999</v>
       </c>
       <c r="S35">
+        <v>50.149000000000001</v>
+      </c>
+      <c r="T35">
+        <v>58.308</v>
+      </c>
+      <c r="U35">
+        <v>64.08</v>
+      </c>
+      <c r="V35">
+        <v>65.472999999999999</v>
+      </c>
+      <c r="W35">
         <v>54.776000000000003</v>
       </c>
-      <c r="T35">
-        <v>55.97</v>
-      </c>
-      <c r="U35">
-        <v>63.482999999999997</v>
-      </c>
-      <c r="V35">
-        <v>63.93</v>
-      </c>
-      <c r="W35">
-        <v>54.627000000000002</v>
-      </c>
       <c r="X35">
-        <v>34.527000000000001</v>
+        <v>34.725999999999999</v>
       </c>
       <c r="Y35">
-        <v>31.890999999999998</v>
+        <v>45.671999999999997</v>
       </c>
       <c r="Z35">
-        <v>50.646999999999998</v>
+        <v>66.617000000000004</v>
       </c>
       <c r="AA35">
-        <v>60.198999999999998</v>
+        <v>78.457999999999998</v>
       </c>
       <c r="AB35">
-        <v>77.611999999999995</v>
+        <v>90.697000000000003</v>
       </c>
       <c r="AC35">
-        <v>97.91</v>
+        <v>109.55200000000001</v>
       </c>
       <c r="AD35">
-        <v>102.09</v>
+        <v>111.194</v>
       </c>
       <c r="AE35">
-        <v>103.333</v>
+        <v>84.924999999999997</v>
       </c>
       <c r="AF35">
-        <v>89.9</v>
+        <v>59.154000000000003</v>
       </c>
       <c r="AG35">
-        <v>48.656999999999996</v>
+        <v>32.04</v>
       </c>
     </row>
     <row r="36" spans="1:33" x14ac:dyDescent="0.45">
@@ -4061,100 +4067,100 @@
         <v>24</v>
       </c>
       <c r="B36">
-        <v>2012</v>
+        <v>63</v>
       </c>
       <c r="C36" t="s">
         <v>43</v>
       </c>
       <c r="D36" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="E36" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F36">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="G36">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H36">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="I36">
-        <v>67.42</v>
+        <v>86</v>
       </c>
       <c r="J36">
-        <v>82.58</v>
+        <v>77.38</v>
       </c>
       <c r="K36">
-        <v>58.12</v>
+        <v>38.17</v>
       </c>
       <c r="L36">
-        <v>34.6</v>
+        <v>33.880000000000003</v>
       </c>
       <c r="M36">
-        <v>73.569999999999993</v>
+        <v>44.81</v>
       </c>
       <c r="N36">
-        <v>51.2</v>
+        <v>30.86</v>
       </c>
       <c r="O36">
-        <v>178.90999999999997</v>
+        <v>175.87</v>
       </c>
       <c r="P36">
-        <v>18.507000000000001</v>
+        <v>18.657</v>
       </c>
       <c r="Q36">
-        <v>36.965000000000003</v>
+        <v>31.193999999999999</v>
       </c>
       <c r="R36">
-        <v>48.408000000000001</v>
+        <v>39.353000000000002</v>
       </c>
       <c r="S36">
+        <v>45.820999999999998</v>
+      </c>
+      <c r="T36">
+        <v>51.890999999999998</v>
+      </c>
+      <c r="U36">
+        <v>54.328000000000003</v>
+      </c>
+      <c r="V36">
+        <v>50.497999999999998</v>
+      </c>
+      <c r="W36">
+        <v>41.143999999999998</v>
+      </c>
+      <c r="X36">
+        <v>28.657</v>
+      </c>
+      <c r="Y36">
+        <v>26.219000000000001</v>
+      </c>
+      <c r="Z36">
+        <v>35.572000000000003</v>
+      </c>
+      <c r="AA36">
         <v>54.776000000000003</v>
       </c>
-      <c r="T36">
-        <v>75.721000000000004</v>
-      </c>
-      <c r="U36">
-        <v>95.622</v>
-      </c>
-      <c r="V36">
-        <v>82.388000000000005</v>
-      </c>
-      <c r="W36">
-        <v>59.552</v>
-      </c>
-      <c r="X36">
-        <v>39.9</v>
-      </c>
-      <c r="Y36">
-        <v>32.735999999999997</v>
-      </c>
-      <c r="Z36">
-        <v>58.01</v>
-      </c>
-      <c r="AA36">
-        <v>78.108999999999995</v>
-      </c>
       <c r="AB36">
-        <v>85.174000000000007</v>
+        <v>66.715999999999994</v>
       </c>
       <c r="AC36">
-        <v>84.179000000000002</v>
+        <v>83.483000000000004</v>
       </c>
       <c r="AD36">
-        <v>81.244</v>
+        <v>91.492999999999995</v>
       </c>
       <c r="AE36">
-        <v>70.796000000000006</v>
+        <v>93.483000000000004</v>
       </c>
       <c r="AF36">
-        <v>58.259</v>
+        <v>82.885999999999996</v>
       </c>
       <c r="AG36">
-        <v>46.816000000000003</v>
+        <v>62.735999999999997</v>
       </c>
     </row>
     <row r="37" spans="1:33" x14ac:dyDescent="0.45">
@@ -4162,103 +4168,912 @@
         <v>24</v>
       </c>
       <c r="B37">
-        <v>2042</v>
+        <v>74</v>
       </c>
       <c r="C37" t="s">
         <v>38</v>
       </c>
       <c r="D37" t="s">
+        <v>39</v>
+      </c>
+      <c r="E37" t="s">
+        <v>41</v>
+      </c>
+      <c r="F37">
+        <v>150</v>
+      </c>
+      <c r="G37">
+        <v>90</v>
+      </c>
+      <c r="H37">
+        <v>73</v>
+      </c>
+      <c r="I37">
+        <v>86.88</v>
+      </c>
+      <c r="J37">
+        <v>73.77</v>
+      </c>
+      <c r="K37">
+        <v>44.09</v>
+      </c>
+      <c r="L37">
+        <v>70.150000000000006</v>
+      </c>
+      <c r="M37">
+        <v>57.66</v>
+      </c>
+      <c r="N37">
+        <v>35.18</v>
+      </c>
+      <c r="O37">
+        <v>167.86</v>
+      </c>
+      <c r="P37">
+        <v>20.646999999999998</v>
+      </c>
+      <c r="Q37">
+        <v>31.244</v>
+      </c>
+      <c r="R37">
+        <v>39.103999999999999</v>
+      </c>
+      <c r="S37">
+        <v>45.572000000000003</v>
+      </c>
+      <c r="T37">
+        <v>58.656999999999996</v>
+      </c>
+      <c r="U37">
+        <v>65.322999999999993</v>
+      </c>
+      <c r="V37">
+        <v>70.995000000000005</v>
+      </c>
+      <c r="W37">
+        <v>74.924999999999997</v>
+      </c>
+      <c r="X37">
+        <v>65.671999999999997</v>
+      </c>
+      <c r="Y37">
+        <v>31.99</v>
+      </c>
+      <c r="Z37">
+        <v>41.293999999999997</v>
+      </c>
+      <c r="AA37">
+        <v>56.119</v>
+      </c>
+      <c r="AB37">
+        <v>70.944999999999993</v>
+      </c>
+      <c r="AC37">
+        <v>80.596999999999994</v>
+      </c>
+      <c r="AD37">
+        <v>93.134</v>
+      </c>
+      <c r="AE37">
+        <v>95.870999999999995</v>
+      </c>
+      <c r="AF37">
+        <v>91.691999999999993</v>
+      </c>
+      <c r="AG37">
+        <v>72.686999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38">
+        <v>102</v>
+      </c>
+      <c r="C38" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38" t="s">
+        <v>39</v>
+      </c>
+      <c r="E38" t="s">
+        <v>42</v>
+      </c>
+      <c r="F38">
+        <v>129</v>
+      </c>
+      <c r="G38">
+        <v>81</v>
+      </c>
+      <c r="H38">
+        <v>46</v>
+      </c>
+      <c r="I38">
+        <v>67.55</v>
+      </c>
+      <c r="J38">
+        <v>79.849999999999994</v>
+      </c>
+      <c r="K38">
+        <v>51.46</v>
+      </c>
+      <c r="L38">
+        <v>28.58</v>
+      </c>
+      <c r="M38">
+        <v>43.38</v>
+      </c>
+      <c r="N38">
+        <v>36.07</v>
+      </c>
+      <c r="O38">
+        <v>135.92000000000002</v>
+      </c>
+      <c r="P38">
+        <v>17.91</v>
+      </c>
+      <c r="Q38">
+        <v>31.591999999999999</v>
+      </c>
+      <c r="R38">
+        <v>39.353000000000002</v>
+      </c>
+      <c r="S38">
+        <v>47.463000000000001</v>
+      </c>
+      <c r="T38">
+        <v>52.387999999999998</v>
+      </c>
+      <c r="U38">
+        <v>51.841000000000001</v>
+      </c>
+      <c r="V38">
+        <v>46.317999999999998</v>
+      </c>
+      <c r="W38">
+        <v>34.776000000000003</v>
+      </c>
+      <c r="X38">
+        <v>19.204000000000001</v>
+      </c>
+      <c r="Y38">
+        <v>20.696999999999999</v>
+      </c>
+      <c r="Z38">
+        <v>38.209000000000003</v>
+      </c>
+      <c r="AA38">
+        <v>66.269000000000005</v>
+      </c>
+      <c r="AB38">
+        <v>76.069999999999993</v>
+      </c>
+      <c r="AC38">
+        <v>80</v>
+      </c>
+      <c r="AD38">
+        <v>75.522000000000006</v>
+      </c>
+      <c r="AE38">
+        <v>73.781000000000006</v>
+      </c>
+      <c r="AF38">
+        <v>66.516999999999996</v>
+      </c>
+      <c r="AG38">
+        <v>53.433</v>
+      </c>
+    </row>
+    <row r="39" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>24</v>
+      </c>
+      <c r="B39">
+        <v>110</v>
+      </c>
+      <c r="C39" t="s">
+        <v>43</v>
+      </c>
+      <c r="D39" t="s">
+        <v>44</v>
+      </c>
+      <c r="E39" t="s">
+        <v>40</v>
+      </c>
+      <c r="F39">
+        <v>119</v>
+      </c>
+      <c r="G39">
+        <v>93</v>
+      </c>
+      <c r="H39">
+        <v>46</v>
+      </c>
+      <c r="I39">
+        <v>93.24</v>
+      </c>
+      <c r="J39">
+        <v>83.59</v>
+      </c>
+      <c r="K39">
+        <v>52.3</v>
+      </c>
+      <c r="L39">
+        <v>45.31</v>
+      </c>
+      <c r="M39">
+        <v>31.4</v>
+      </c>
+      <c r="N39">
+        <v>18.54</v>
+      </c>
+      <c r="O39">
+        <v>124.69</v>
+      </c>
+      <c r="P39">
+        <v>15.111000000000001</v>
+      </c>
+      <c r="Q39">
+        <v>25.382999999999999</v>
+      </c>
+      <c r="R39">
+        <v>33.481000000000002</v>
+      </c>
+      <c r="S39">
+        <v>43.604999999999997</v>
+      </c>
+      <c r="T39">
+        <v>51.16</v>
+      </c>
+      <c r="U39">
+        <v>58.863999999999997</v>
+      </c>
+      <c r="V39">
+        <v>61.728000000000002</v>
+      </c>
+      <c r="W39">
+        <v>50.37</v>
+      </c>
+      <c r="X39">
+        <v>36.148000000000003</v>
+      </c>
+      <c r="Y39">
+        <v>34.469000000000001</v>
+      </c>
+      <c r="Z39">
+        <v>47.654000000000003</v>
+      </c>
+      <c r="AA39">
+        <v>59.357999999999997</v>
+      </c>
+      <c r="AB39">
+        <v>68.988</v>
+      </c>
+      <c r="AC39">
+        <v>88.84</v>
+      </c>
+      <c r="AD39">
+        <v>90.123000000000005</v>
+      </c>
+      <c r="AE39">
+        <v>93.826999999999998</v>
+      </c>
+      <c r="AF39">
+        <v>88.938000000000002</v>
+      </c>
+      <c r="AG39">
+        <v>76.494</v>
+      </c>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>24</v>
+      </c>
+      <c r="B40">
+        <v>113</v>
+      </c>
+      <c r="C40" t="s">
+        <v>43</v>
+      </c>
+      <c r="D40" t="s">
+        <v>44</v>
+      </c>
+      <c r="E40" t="s">
+        <v>49</v>
+      </c>
+      <c r="F40">
+        <v>126</v>
+      </c>
+      <c r="G40">
+        <v>80.62</v>
+      </c>
+      <c r="H40">
+        <v>42</v>
+      </c>
+      <c r="I40">
+        <v>47</v>
+      </c>
+      <c r="J40">
+        <v>78</v>
+      </c>
+      <c r="K40">
+        <v>48.6</v>
+      </c>
+      <c r="L40">
+        <v>41.22</v>
+      </c>
+      <c r="M40">
+        <v>40.369999999999997</v>
+      </c>
+      <c r="N40">
+        <v>20.329999999999998</v>
+      </c>
+      <c r="O40">
+        <v>136.15</v>
+      </c>
+      <c r="P40">
+        <v>14.37</v>
+      </c>
+      <c r="Q40">
+        <v>24.542999999999999</v>
+      </c>
+      <c r="R40">
+        <v>32.148000000000003</v>
+      </c>
+      <c r="S40">
+        <v>38.518999999999998</v>
+      </c>
+      <c r="T40">
+        <v>44.84</v>
+      </c>
+      <c r="U40">
+        <v>50.963000000000001</v>
+      </c>
+      <c r="V40">
+        <v>55.802</v>
+      </c>
+      <c r="W40">
+        <v>40.295999999999999</v>
+      </c>
+      <c r="X40">
+        <v>23.259</v>
+      </c>
+      <c r="Y40">
+        <v>27.407</v>
+      </c>
+      <c r="Z40">
+        <v>47.061999999999998</v>
+      </c>
+      <c r="AA40">
+        <v>65.284000000000006</v>
+      </c>
+      <c r="AB40">
+        <v>77.234999999999999</v>
+      </c>
+      <c r="AC40">
+        <v>79.555999999999997</v>
+      </c>
+      <c r="AD40">
+        <v>81.135999999999996</v>
+      </c>
+      <c r="AE40">
+        <v>73.234999999999999</v>
+      </c>
+      <c r="AF40">
+        <v>59.357999999999997</v>
+      </c>
+      <c r="AG40">
+        <v>38.024999999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>24</v>
+      </c>
+      <c r="B41">
+        <v>114</v>
+      </c>
+      <c r="C41" t="s">
+        <v>38</v>
+      </c>
+      <c r="D41" t="s">
+        <v>46</v>
+      </c>
+      <c r="E41" t="s">
+        <v>41</v>
+      </c>
+      <c r="F41">
+        <v>115</v>
+      </c>
+      <c r="G41">
+        <v>78</v>
+      </c>
+      <c r="H41">
+        <v>42</v>
+      </c>
+      <c r="I41">
+        <v>73.87</v>
+      </c>
+      <c r="J41">
+        <v>71.33</v>
+      </c>
+      <c r="K41">
+        <v>61.77</v>
+      </c>
+      <c r="L41">
+        <v>50.99</v>
+      </c>
+      <c r="M41">
+        <v>49.98</v>
+      </c>
+      <c r="N41">
+        <v>32.04</v>
+      </c>
+      <c r="O41">
+        <v>119.85</v>
+      </c>
+      <c r="P41">
+        <v>19.012</v>
+      </c>
+      <c r="Q41">
+        <v>36.691000000000003</v>
+      </c>
+      <c r="R41">
+        <v>42.814999999999998</v>
+      </c>
+      <c r="S41">
+        <v>49.728000000000002</v>
+      </c>
+      <c r="T41">
+        <v>50.469000000000001</v>
+      </c>
+      <c r="U41">
+        <v>53.383000000000003</v>
+      </c>
+      <c r="V41">
+        <v>55.16</v>
+      </c>
+      <c r="W41">
+        <v>50.716000000000001</v>
+      </c>
+      <c r="X41">
+        <v>40.840000000000003</v>
+      </c>
+      <c r="Y41">
+        <v>21.283999999999999</v>
+      </c>
+      <c r="Z41">
+        <v>36.840000000000003</v>
+      </c>
+      <c r="AA41">
+        <v>48.542999999999999</v>
+      </c>
+      <c r="AB41">
+        <v>60.098999999999997</v>
+      </c>
+      <c r="AC41">
+        <v>70.962999999999994</v>
+      </c>
+      <c r="AD41">
+        <v>77.382999999999996</v>
+      </c>
+      <c r="AE41">
+        <v>74.221999999999994</v>
+      </c>
+      <c r="AF41">
+        <v>65.284000000000006</v>
+      </c>
+      <c r="AG41">
+        <v>49.877000000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42">
+        <v>115</v>
+      </c>
+      <c r="C42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D42" t="s">
+        <v>44</v>
+      </c>
+      <c r="E42" t="s">
+        <v>40</v>
+      </c>
+      <c r="F42">
+        <v>121</v>
+      </c>
+      <c r="G42">
+        <v>114</v>
+      </c>
+      <c r="H42">
+        <v>50</v>
+      </c>
+      <c r="I42">
+        <v>82.95</v>
+      </c>
+      <c r="J42">
+        <v>99.37</v>
+      </c>
+      <c r="K42">
+        <v>67.2</v>
+      </c>
+      <c r="L42">
+        <v>47.05</v>
+      </c>
+      <c r="M42">
+        <v>44.63</v>
+      </c>
+      <c r="N42">
+        <v>27.15</v>
+      </c>
+      <c r="O42">
+        <v>154.57</v>
+      </c>
+      <c r="P42">
+        <v>12.542999999999999</v>
+      </c>
+      <c r="Q42">
+        <v>22.617000000000001</v>
+      </c>
+      <c r="R42">
+        <v>32.691000000000003</v>
+      </c>
+      <c r="S42">
+        <v>40.542999999999999</v>
+      </c>
+      <c r="T42">
+        <v>48.247</v>
+      </c>
+      <c r="U42">
+        <v>51.704000000000001</v>
+      </c>
+      <c r="V42">
+        <v>52.098999999999997</v>
+      </c>
+      <c r="W42">
+        <v>53.877000000000002</v>
+      </c>
+      <c r="X42">
+        <v>47.259</v>
+      </c>
+      <c r="Y42">
+        <v>35.061999999999998</v>
+      </c>
+      <c r="Z42">
+        <v>63.110999999999997</v>
+      </c>
+      <c r="AA42">
+        <v>77.974999999999994</v>
+      </c>
+      <c r="AB42">
+        <v>97.135999999999996</v>
+      </c>
+      <c r="AC42">
+        <v>99.259</v>
+      </c>
+      <c r="AD42">
+        <v>96.494</v>
+      </c>
+      <c r="AE42">
+        <v>90.715999999999994</v>
+      </c>
+      <c r="AF42">
+        <v>81.480999999999995</v>
+      </c>
+      <c r="AG42">
+        <v>70.765000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43">
+        <v>226</v>
+      </c>
+      <c r="C43" t="s">
+        <v>43</v>
+      </c>
+      <c r="D43" t="s">
         <v>51</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E43" t="s">
         <v>42</v>
       </c>
-      <c r="F37">
+      <c r="F43">
+        <v>156</v>
+      </c>
+      <c r="G43">
+        <v>106</v>
+      </c>
+      <c r="H43">
+        <v>57</v>
+      </c>
+      <c r="I43">
+        <v>96.86</v>
+      </c>
+      <c r="J43">
+        <v>90.31</v>
+      </c>
+      <c r="K43">
+        <v>50.24</v>
+      </c>
+      <c r="L43">
+        <v>50.41</v>
+      </c>
+      <c r="M43">
+        <v>55</v>
+      </c>
+      <c r="N43">
+        <v>26.4</v>
+      </c>
+      <c r="O43">
+        <v>159.80000000000001</v>
+      </c>
+      <c r="P43">
+        <v>22.934999999999999</v>
+      </c>
+      <c r="Q43">
+        <v>38.408000000000001</v>
+      </c>
+      <c r="R43">
+        <v>50.298999999999999</v>
+      </c>
+      <c r="S43">
+        <v>54.776000000000003</v>
+      </c>
+      <c r="T43">
+        <v>55.97</v>
+      </c>
+      <c r="U43">
+        <v>63.482999999999997</v>
+      </c>
+      <c r="V43">
+        <v>63.93</v>
+      </c>
+      <c r="W43">
+        <v>54.627000000000002</v>
+      </c>
+      <c r="X43">
+        <v>34.527000000000001</v>
+      </c>
+      <c r="Y43">
+        <v>31.890999999999998</v>
+      </c>
+      <c r="Z43">
+        <v>50.646999999999998</v>
+      </c>
+      <c r="AA43">
+        <v>60.198999999999998</v>
+      </c>
+      <c r="AB43">
+        <v>77.611999999999995</v>
+      </c>
+      <c r="AC43">
+        <v>97.91</v>
+      </c>
+      <c r="AD43">
+        <v>102.09</v>
+      </c>
+      <c r="AE43">
+        <v>103.333</v>
+      </c>
+      <c r="AF43">
+        <v>89.9</v>
+      </c>
+      <c r="AG43">
+        <v>48.656999999999996</v>
+      </c>
+    </row>
+    <row r="44" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>24</v>
+      </c>
+      <c r="B44">
+        <v>2012</v>
+      </c>
+      <c r="C44" t="s">
+        <v>43</v>
+      </c>
+      <c r="D44" t="s">
+        <v>39</v>
+      </c>
+      <c r="E44" t="s">
+        <v>42</v>
+      </c>
+      <c r="F44">
+        <v>174</v>
+      </c>
+      <c r="G44">
+        <v>84</v>
+      </c>
+      <c r="H44">
+        <v>75</v>
+      </c>
+      <c r="I44">
+        <v>67.42</v>
+      </c>
+      <c r="J44">
+        <v>82.58</v>
+      </c>
+      <c r="K44">
+        <v>58.12</v>
+      </c>
+      <c r="L44">
+        <v>34.6</v>
+      </c>
+      <c r="M44">
+        <v>73.569999999999993</v>
+      </c>
+      <c r="N44">
+        <v>51.2</v>
+      </c>
+      <c r="O44">
+        <v>178.90999999999997</v>
+      </c>
+      <c r="P44">
+        <v>18.507000000000001</v>
+      </c>
+      <c r="Q44">
+        <v>36.965000000000003</v>
+      </c>
+      <c r="R44">
+        <v>48.408000000000001</v>
+      </c>
+      <c r="S44">
+        <v>54.776000000000003</v>
+      </c>
+      <c r="T44">
+        <v>75.721000000000004</v>
+      </c>
+      <c r="U44">
+        <v>95.622</v>
+      </c>
+      <c r="V44">
+        <v>82.388000000000005</v>
+      </c>
+      <c r="W44">
+        <v>59.552</v>
+      </c>
+      <c r="X44">
+        <v>39.9</v>
+      </c>
+      <c r="Y44">
+        <v>32.735999999999997</v>
+      </c>
+      <c r="Z44">
+        <v>58.01</v>
+      </c>
+      <c r="AA44">
+        <v>78.108999999999995</v>
+      </c>
+      <c r="AB44">
+        <v>85.174000000000007</v>
+      </c>
+      <c r="AC44">
+        <v>84.179000000000002</v>
+      </c>
+      <c r="AD44">
+        <v>81.244</v>
+      </c>
+      <c r="AE44">
+        <v>70.796000000000006</v>
+      </c>
+      <c r="AF44">
+        <v>58.259</v>
+      </c>
+      <c r="AG44">
+        <v>46.816000000000003</v>
+      </c>
+    </row>
+    <row r="45" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>24</v>
+      </c>
+      <c r="B45">
+        <v>2042</v>
+      </c>
+      <c r="C45" t="s">
+        <v>38</v>
+      </c>
+      <c r="D45" t="s">
+        <v>51</v>
+      </c>
+      <c r="E45" t="s">
+        <v>42</v>
+      </c>
+      <c r="F45">
         <v>158</v>
       </c>
-      <c r="G37">
+      <c r="G45">
         <v>86</v>
       </c>
-      <c r="H37">
+      <c r="H45">
         <v>60</v>
       </c>
-      <c r="I37">
+      <c r="I45">
         <v>64.739999999999995</v>
       </c>
-      <c r="J37">
+      <c r="J45">
         <v>84.12</v>
       </c>
-      <c r="K37">
+      <c r="K45">
         <v>58.27</v>
       </c>
-      <c r="L37">
+      <c r="L45">
         <v>39.54</v>
       </c>
-      <c r="M37">
+      <c r="M45">
         <v>60</v>
       </c>
-      <c r="N37">
+      <c r="N45">
         <v>25.41</v>
       </c>
-      <c r="O37">
+      <c r="O45">
         <v>168.46</v>
       </c>
-      <c r="P37">
+      <c r="P45">
         <v>15.622</v>
       </c>
-      <c r="Q37">
+      <c r="Q45">
         <v>34.328000000000003</v>
       </c>
-      <c r="R37">
+      <c r="R45">
         <v>58.109000000000002</v>
       </c>
-      <c r="S37">
+      <c r="S45">
         <v>60.697000000000003</v>
       </c>
-      <c r="T37">
+      <c r="T45">
         <v>61.692</v>
       </c>
-      <c r="U37">
+      <c r="U45">
         <v>63.085000000000001</v>
       </c>
-      <c r="V37">
+      <c r="V45">
         <v>62.786000000000001</v>
       </c>
-      <c r="W37">
+      <c r="W45">
         <v>53.731000000000002</v>
       </c>
-      <c r="X37">
+      <c r="X45">
         <v>42.289000000000001</v>
       </c>
-      <c r="Y37">
+      <c r="Y45">
         <v>41.542000000000002</v>
       </c>
-      <c r="Z37">
+      <c r="Z45">
         <v>53.631999999999998</v>
       </c>
-      <c r="AA37">
+      <c r="AA45">
         <v>73.581999999999994</v>
       </c>
-      <c r="AB37">
+      <c r="AB45">
         <v>77.164000000000001</v>
       </c>
-      <c r="AC37">
+      <c r="AC45">
         <v>86.07</v>
       </c>
-      <c r="AD37">
+      <c r="AD45">
         <v>79.004999999999995</v>
       </c>
-      <c r="AE37">
+      <c r="AE45">
         <v>70.596999999999994</v>
       </c>
-      <c r="AF37">
+      <c r="AF45">
         <v>60.398000000000003</v>
       </c>
-      <c r="AG37">
+      <c r="AG45">
         <v>42.488</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>